<commit_message>
tfs2249 - ecl csr survey text changes
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C34057
</commit_message>
<xml_diff>
--- a/Requirements/CCO_eCoaching_Log_Survey_Questions.xlsx
+++ b/Requirements/CCO_eCoaching_Log_Survey_Questions.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Requirements\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="2" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>Survey Question</t>
   </si>
@@ -61,13 +66,7 @@
     <t>Follow up</t>
   </si>
   <si>
-    <t>If yes, how?  If no, why  not?</t>
-  </si>
-  <si>
     <t>If no, what reason was provided?</t>
-  </si>
-  <si>
-    <t>If yes, what specifically.  If no, why not?</t>
   </si>
   <si>
     <t>Please explain below.</t>
@@ -126,6 +125,15 @@
   </si>
   <si>
     <t>End Date</t>
+  </si>
+  <si>
+    <t>If yes, how?  If no, what suggestions or recommendations could have made it more useful for you?</t>
+  </si>
+  <si>
+    <t>TFS2249 - eCL CSR Survey text changes (modified follow up for questions 2 and 3</t>
+  </si>
+  <si>
+    <t>If yes, what specifically?  If no, what could have made it more effective or valuable?</t>
   </si>
 </sst>
 </file>
@@ -230,6 +238,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -277,7 +288,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -312,7 +323,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -523,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,16 +864,16 @@
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -870,20 +881,28 @@
         <v>42255</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="11">
         <v>1</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="10"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>42451</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="11">
+        <v>1.01</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
@@ -1188,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>7</v>
@@ -1226,10 +1245,10 @@
         <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1240,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -1249,7 +1268,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -1258,7 +1277,7 @@
         <v>42255</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1272,10 +1291,10 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -1284,7 +1303,7 @@
         <v>42255</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1292,16 +1311,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -1318,16 +1337,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
@@ -1344,7 +1363,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -1353,7 +1372,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
@@ -1390,13 +1409,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -1408,7 +1427,7 @@
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tfs9511 - ecl pilot survey question
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C39394
</commit_message>
<xml_diff>
--- a/Requirements/CCO_eCoaching_Log_Survey_Questions.xlsx
+++ b/Requirements/CCO_eCoaching_Log_Survey_Questions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="72" windowWidth="18192" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="46">
   <si>
     <t>Survey Question</t>
   </si>
@@ -134,6 +134,51 @@
   </si>
   <si>
     <t>If yes, what specifically?  If no, what could have made it more effective or valuable?</t>
+  </si>
+  <si>
+    <t>How prepared was your supervisor during your coaching session?</t>
+  </si>
+  <si>
+    <t>1 - Very Prepared
+2 - Prepared
+3 - Neither Prepared or Unprepared
+4 - Unprepared
+5 - Very Unprepared</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Lawrence</t>
+  </si>
+  <si>
+    <t>Eligible Logs</t>
+  </si>
+  <si>
+    <t>All except Verint-TQC source</t>
+  </si>
+  <si>
+    <t>Coaching Reasons of
+Call Efficiency
+CCO Processes and Procedures
+Current Coaching Initiative 
+HR Guidelines Issue
+Quality
+Recognition
+Secure Floor Violations</t>
+  </si>
+  <si>
+    <t>is Hot Topic</t>
+  </si>
+  <si>
+    <t>is Pilot</t>
+  </si>
+  <si>
+    <t>TFS6511 - eCL Pilot Survey Question
+Added new question for Lawrence, columns for eligible logs, hot topic and pilot</t>
   </si>
 </sst>
 </file>
@@ -188,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -226,6 +271,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -534,335 +582,335 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="40.109375" style="14" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="257" max="257" width="9.140625" customWidth="1"/>
-    <col min="258" max="258" width="15.42578125" customWidth="1"/>
-    <col min="259" max="259" width="40.140625" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="257" max="257" width="9.109375" customWidth="1"/>
+    <col min="258" max="258" width="15.44140625" customWidth="1"/>
+    <col min="259" max="259" width="40.109375" customWidth="1"/>
     <col min="260" max="260" width="22" customWidth="1"/>
-    <col min="261" max="261" width="25.7109375" customWidth="1"/>
-    <col min="513" max="513" width="9.140625" customWidth="1"/>
-    <col min="514" max="514" width="15.42578125" customWidth="1"/>
-    <col min="515" max="515" width="40.140625" customWidth="1"/>
+    <col min="261" max="261" width="25.6640625" customWidth="1"/>
+    <col min="513" max="513" width="9.109375" customWidth="1"/>
+    <col min="514" max="514" width="15.44140625" customWidth="1"/>
+    <col min="515" max="515" width="40.109375" customWidth="1"/>
     <col min="516" max="516" width="22" customWidth="1"/>
-    <col min="517" max="517" width="25.7109375" customWidth="1"/>
-    <col min="769" max="769" width="9.140625" customWidth="1"/>
-    <col min="770" max="770" width="15.42578125" customWidth="1"/>
-    <col min="771" max="771" width="40.140625" customWidth="1"/>
+    <col min="517" max="517" width="25.6640625" customWidth="1"/>
+    <col min="769" max="769" width="9.109375" customWidth="1"/>
+    <col min="770" max="770" width="15.44140625" customWidth="1"/>
+    <col min="771" max="771" width="40.109375" customWidth="1"/>
     <col min="772" max="772" width="22" customWidth="1"/>
-    <col min="773" max="773" width="25.7109375" customWidth="1"/>
-    <col min="1025" max="1025" width="9.140625" customWidth="1"/>
-    <col min="1026" max="1026" width="15.42578125" customWidth="1"/>
-    <col min="1027" max="1027" width="40.140625" customWidth="1"/>
+    <col min="773" max="773" width="25.6640625" customWidth="1"/>
+    <col min="1025" max="1025" width="9.109375" customWidth="1"/>
+    <col min="1026" max="1026" width="15.44140625" customWidth="1"/>
+    <col min="1027" max="1027" width="40.109375" customWidth="1"/>
     <col min="1028" max="1028" width="22" customWidth="1"/>
-    <col min="1029" max="1029" width="25.7109375" customWidth="1"/>
-    <col min="1281" max="1281" width="9.140625" customWidth="1"/>
-    <col min="1282" max="1282" width="15.42578125" customWidth="1"/>
-    <col min="1283" max="1283" width="40.140625" customWidth="1"/>
+    <col min="1029" max="1029" width="25.6640625" customWidth="1"/>
+    <col min="1281" max="1281" width="9.109375" customWidth="1"/>
+    <col min="1282" max="1282" width="15.44140625" customWidth="1"/>
+    <col min="1283" max="1283" width="40.109375" customWidth="1"/>
     <col min="1284" max="1284" width="22" customWidth="1"/>
-    <col min="1285" max="1285" width="25.7109375" customWidth="1"/>
-    <col min="1537" max="1537" width="9.140625" customWidth="1"/>
-    <col min="1538" max="1538" width="15.42578125" customWidth="1"/>
-    <col min="1539" max="1539" width="40.140625" customWidth="1"/>
+    <col min="1285" max="1285" width="25.6640625" customWidth="1"/>
+    <col min="1537" max="1537" width="9.109375" customWidth="1"/>
+    <col min="1538" max="1538" width="15.44140625" customWidth="1"/>
+    <col min="1539" max="1539" width="40.109375" customWidth="1"/>
     <col min="1540" max="1540" width="22" customWidth="1"/>
-    <col min="1541" max="1541" width="25.7109375" customWidth="1"/>
-    <col min="1793" max="1793" width="9.140625" customWidth="1"/>
-    <col min="1794" max="1794" width="15.42578125" customWidth="1"/>
-    <col min="1795" max="1795" width="40.140625" customWidth="1"/>
+    <col min="1541" max="1541" width="25.6640625" customWidth="1"/>
+    <col min="1793" max="1793" width="9.109375" customWidth="1"/>
+    <col min="1794" max="1794" width="15.44140625" customWidth="1"/>
+    <col min="1795" max="1795" width="40.109375" customWidth="1"/>
     <col min="1796" max="1796" width="22" customWidth="1"/>
-    <col min="1797" max="1797" width="25.7109375" customWidth="1"/>
-    <col min="2049" max="2049" width="9.140625" customWidth="1"/>
-    <col min="2050" max="2050" width="15.42578125" customWidth="1"/>
-    <col min="2051" max="2051" width="40.140625" customWidth="1"/>
+    <col min="1797" max="1797" width="25.6640625" customWidth="1"/>
+    <col min="2049" max="2049" width="9.109375" customWidth="1"/>
+    <col min="2050" max="2050" width="15.44140625" customWidth="1"/>
+    <col min="2051" max="2051" width="40.109375" customWidth="1"/>
     <col min="2052" max="2052" width="22" customWidth="1"/>
-    <col min="2053" max="2053" width="25.7109375" customWidth="1"/>
-    <col min="2305" max="2305" width="9.140625" customWidth="1"/>
-    <col min="2306" max="2306" width="15.42578125" customWidth="1"/>
-    <col min="2307" max="2307" width="40.140625" customWidth="1"/>
+    <col min="2053" max="2053" width="25.6640625" customWidth="1"/>
+    <col min="2305" max="2305" width="9.109375" customWidth="1"/>
+    <col min="2306" max="2306" width="15.44140625" customWidth="1"/>
+    <col min="2307" max="2307" width="40.109375" customWidth="1"/>
     <col min="2308" max="2308" width="22" customWidth="1"/>
-    <col min="2309" max="2309" width="25.7109375" customWidth="1"/>
-    <col min="2561" max="2561" width="9.140625" customWidth="1"/>
-    <col min="2562" max="2562" width="15.42578125" customWidth="1"/>
-    <col min="2563" max="2563" width="40.140625" customWidth="1"/>
+    <col min="2309" max="2309" width="25.6640625" customWidth="1"/>
+    <col min="2561" max="2561" width="9.109375" customWidth="1"/>
+    <col min="2562" max="2562" width="15.44140625" customWidth="1"/>
+    <col min="2563" max="2563" width="40.109375" customWidth="1"/>
     <col min="2564" max="2564" width="22" customWidth="1"/>
-    <col min="2565" max="2565" width="25.7109375" customWidth="1"/>
-    <col min="2817" max="2817" width="9.140625" customWidth="1"/>
-    <col min="2818" max="2818" width="15.42578125" customWidth="1"/>
-    <col min="2819" max="2819" width="40.140625" customWidth="1"/>
+    <col min="2565" max="2565" width="25.6640625" customWidth="1"/>
+    <col min="2817" max="2817" width="9.109375" customWidth="1"/>
+    <col min="2818" max="2818" width="15.44140625" customWidth="1"/>
+    <col min="2819" max="2819" width="40.109375" customWidth="1"/>
     <col min="2820" max="2820" width="22" customWidth="1"/>
-    <col min="2821" max="2821" width="25.7109375" customWidth="1"/>
-    <col min="3073" max="3073" width="9.140625" customWidth="1"/>
-    <col min="3074" max="3074" width="15.42578125" customWidth="1"/>
-    <col min="3075" max="3075" width="40.140625" customWidth="1"/>
+    <col min="2821" max="2821" width="25.6640625" customWidth="1"/>
+    <col min="3073" max="3073" width="9.109375" customWidth="1"/>
+    <col min="3074" max="3074" width="15.44140625" customWidth="1"/>
+    <col min="3075" max="3075" width="40.109375" customWidth="1"/>
     <col min="3076" max="3076" width="22" customWidth="1"/>
-    <col min="3077" max="3077" width="25.7109375" customWidth="1"/>
-    <col min="3329" max="3329" width="9.140625" customWidth="1"/>
-    <col min="3330" max="3330" width="15.42578125" customWidth="1"/>
-    <col min="3331" max="3331" width="40.140625" customWidth="1"/>
+    <col min="3077" max="3077" width="25.6640625" customWidth="1"/>
+    <col min="3329" max="3329" width="9.109375" customWidth="1"/>
+    <col min="3330" max="3330" width="15.44140625" customWidth="1"/>
+    <col min="3331" max="3331" width="40.109375" customWidth="1"/>
     <col min="3332" max="3332" width="22" customWidth="1"/>
-    <col min="3333" max="3333" width="25.7109375" customWidth="1"/>
-    <col min="3585" max="3585" width="9.140625" customWidth="1"/>
-    <col min="3586" max="3586" width="15.42578125" customWidth="1"/>
-    <col min="3587" max="3587" width="40.140625" customWidth="1"/>
+    <col min="3333" max="3333" width="25.6640625" customWidth="1"/>
+    <col min="3585" max="3585" width="9.109375" customWidth="1"/>
+    <col min="3586" max="3586" width="15.44140625" customWidth="1"/>
+    <col min="3587" max="3587" width="40.109375" customWidth="1"/>
     <col min="3588" max="3588" width="22" customWidth="1"/>
-    <col min="3589" max="3589" width="25.7109375" customWidth="1"/>
-    <col min="3841" max="3841" width="9.140625" customWidth="1"/>
-    <col min="3842" max="3842" width="15.42578125" customWidth="1"/>
-    <col min="3843" max="3843" width="40.140625" customWidth="1"/>
+    <col min="3589" max="3589" width="25.6640625" customWidth="1"/>
+    <col min="3841" max="3841" width="9.109375" customWidth="1"/>
+    <col min="3842" max="3842" width="15.44140625" customWidth="1"/>
+    <col min="3843" max="3843" width="40.109375" customWidth="1"/>
     <col min="3844" max="3844" width="22" customWidth="1"/>
-    <col min="3845" max="3845" width="25.7109375" customWidth="1"/>
-    <col min="4097" max="4097" width="9.140625" customWidth="1"/>
-    <col min="4098" max="4098" width="15.42578125" customWidth="1"/>
-    <col min="4099" max="4099" width="40.140625" customWidth="1"/>
+    <col min="3845" max="3845" width="25.6640625" customWidth="1"/>
+    <col min="4097" max="4097" width="9.109375" customWidth="1"/>
+    <col min="4098" max="4098" width="15.44140625" customWidth="1"/>
+    <col min="4099" max="4099" width="40.109375" customWidth="1"/>
     <col min="4100" max="4100" width="22" customWidth="1"/>
-    <col min="4101" max="4101" width="25.7109375" customWidth="1"/>
-    <col min="4353" max="4353" width="9.140625" customWidth="1"/>
-    <col min="4354" max="4354" width="15.42578125" customWidth="1"/>
-    <col min="4355" max="4355" width="40.140625" customWidth="1"/>
+    <col min="4101" max="4101" width="25.6640625" customWidth="1"/>
+    <col min="4353" max="4353" width="9.109375" customWidth="1"/>
+    <col min="4354" max="4354" width="15.44140625" customWidth="1"/>
+    <col min="4355" max="4355" width="40.109375" customWidth="1"/>
     <col min="4356" max="4356" width="22" customWidth="1"/>
-    <col min="4357" max="4357" width="25.7109375" customWidth="1"/>
-    <col min="4609" max="4609" width="9.140625" customWidth="1"/>
-    <col min="4610" max="4610" width="15.42578125" customWidth="1"/>
-    <col min="4611" max="4611" width="40.140625" customWidth="1"/>
+    <col min="4357" max="4357" width="25.6640625" customWidth="1"/>
+    <col min="4609" max="4609" width="9.109375" customWidth="1"/>
+    <col min="4610" max="4610" width="15.44140625" customWidth="1"/>
+    <col min="4611" max="4611" width="40.109375" customWidth="1"/>
     <col min="4612" max="4612" width="22" customWidth="1"/>
-    <col min="4613" max="4613" width="25.7109375" customWidth="1"/>
-    <col min="4865" max="4865" width="9.140625" customWidth="1"/>
-    <col min="4866" max="4866" width="15.42578125" customWidth="1"/>
-    <col min="4867" max="4867" width="40.140625" customWidth="1"/>
+    <col min="4613" max="4613" width="25.6640625" customWidth="1"/>
+    <col min="4865" max="4865" width="9.109375" customWidth="1"/>
+    <col min="4866" max="4866" width="15.44140625" customWidth="1"/>
+    <col min="4867" max="4867" width="40.109375" customWidth="1"/>
     <col min="4868" max="4868" width="22" customWidth="1"/>
-    <col min="4869" max="4869" width="25.7109375" customWidth="1"/>
-    <col min="5121" max="5121" width="9.140625" customWidth="1"/>
-    <col min="5122" max="5122" width="15.42578125" customWidth="1"/>
-    <col min="5123" max="5123" width="40.140625" customWidth="1"/>
+    <col min="4869" max="4869" width="25.6640625" customWidth="1"/>
+    <col min="5121" max="5121" width="9.109375" customWidth="1"/>
+    <col min="5122" max="5122" width="15.44140625" customWidth="1"/>
+    <col min="5123" max="5123" width="40.109375" customWidth="1"/>
     <col min="5124" max="5124" width="22" customWidth="1"/>
-    <col min="5125" max="5125" width="25.7109375" customWidth="1"/>
-    <col min="5377" max="5377" width="9.140625" customWidth="1"/>
-    <col min="5378" max="5378" width="15.42578125" customWidth="1"/>
-    <col min="5379" max="5379" width="40.140625" customWidth="1"/>
+    <col min="5125" max="5125" width="25.6640625" customWidth="1"/>
+    <col min="5377" max="5377" width="9.109375" customWidth="1"/>
+    <col min="5378" max="5378" width="15.44140625" customWidth="1"/>
+    <col min="5379" max="5379" width="40.109375" customWidth="1"/>
     <col min="5380" max="5380" width="22" customWidth="1"/>
-    <col min="5381" max="5381" width="25.7109375" customWidth="1"/>
-    <col min="5633" max="5633" width="9.140625" customWidth="1"/>
-    <col min="5634" max="5634" width="15.42578125" customWidth="1"/>
-    <col min="5635" max="5635" width="40.140625" customWidth="1"/>
+    <col min="5381" max="5381" width="25.6640625" customWidth="1"/>
+    <col min="5633" max="5633" width="9.109375" customWidth="1"/>
+    <col min="5634" max="5634" width="15.44140625" customWidth="1"/>
+    <col min="5635" max="5635" width="40.109375" customWidth="1"/>
     <col min="5636" max="5636" width="22" customWidth="1"/>
-    <col min="5637" max="5637" width="25.7109375" customWidth="1"/>
-    <col min="5889" max="5889" width="9.140625" customWidth="1"/>
-    <col min="5890" max="5890" width="15.42578125" customWidth="1"/>
-    <col min="5891" max="5891" width="40.140625" customWidth="1"/>
+    <col min="5637" max="5637" width="25.6640625" customWidth="1"/>
+    <col min="5889" max="5889" width="9.109375" customWidth="1"/>
+    <col min="5890" max="5890" width="15.44140625" customWidth="1"/>
+    <col min="5891" max="5891" width="40.109375" customWidth="1"/>
     <col min="5892" max="5892" width="22" customWidth="1"/>
-    <col min="5893" max="5893" width="25.7109375" customWidth="1"/>
-    <col min="6145" max="6145" width="9.140625" customWidth="1"/>
-    <col min="6146" max="6146" width="15.42578125" customWidth="1"/>
-    <col min="6147" max="6147" width="40.140625" customWidth="1"/>
+    <col min="5893" max="5893" width="25.6640625" customWidth="1"/>
+    <col min="6145" max="6145" width="9.109375" customWidth="1"/>
+    <col min="6146" max="6146" width="15.44140625" customWidth="1"/>
+    <col min="6147" max="6147" width="40.109375" customWidth="1"/>
     <col min="6148" max="6148" width="22" customWidth="1"/>
-    <col min="6149" max="6149" width="25.7109375" customWidth="1"/>
-    <col min="6401" max="6401" width="9.140625" customWidth="1"/>
-    <col min="6402" max="6402" width="15.42578125" customWidth="1"/>
-    <col min="6403" max="6403" width="40.140625" customWidth="1"/>
+    <col min="6149" max="6149" width="25.6640625" customWidth="1"/>
+    <col min="6401" max="6401" width="9.109375" customWidth="1"/>
+    <col min="6402" max="6402" width="15.44140625" customWidth="1"/>
+    <col min="6403" max="6403" width="40.109375" customWidth="1"/>
     <col min="6404" max="6404" width="22" customWidth="1"/>
-    <col min="6405" max="6405" width="25.7109375" customWidth="1"/>
-    <col min="6657" max="6657" width="9.140625" customWidth="1"/>
-    <col min="6658" max="6658" width="15.42578125" customWidth="1"/>
-    <col min="6659" max="6659" width="40.140625" customWidth="1"/>
+    <col min="6405" max="6405" width="25.6640625" customWidth="1"/>
+    <col min="6657" max="6657" width="9.109375" customWidth="1"/>
+    <col min="6658" max="6658" width="15.44140625" customWidth="1"/>
+    <col min="6659" max="6659" width="40.109375" customWidth="1"/>
     <col min="6660" max="6660" width="22" customWidth="1"/>
-    <col min="6661" max="6661" width="25.7109375" customWidth="1"/>
-    <col min="6913" max="6913" width="9.140625" customWidth="1"/>
-    <col min="6914" max="6914" width="15.42578125" customWidth="1"/>
-    <col min="6915" max="6915" width="40.140625" customWidth="1"/>
+    <col min="6661" max="6661" width="25.6640625" customWidth="1"/>
+    <col min="6913" max="6913" width="9.109375" customWidth="1"/>
+    <col min="6914" max="6914" width="15.44140625" customWidth="1"/>
+    <col min="6915" max="6915" width="40.109375" customWidth="1"/>
     <col min="6916" max="6916" width="22" customWidth="1"/>
-    <col min="6917" max="6917" width="25.7109375" customWidth="1"/>
-    <col min="7169" max="7169" width="9.140625" customWidth="1"/>
-    <col min="7170" max="7170" width="15.42578125" customWidth="1"/>
-    <col min="7171" max="7171" width="40.140625" customWidth="1"/>
+    <col min="6917" max="6917" width="25.6640625" customWidth="1"/>
+    <col min="7169" max="7169" width="9.109375" customWidth="1"/>
+    <col min="7170" max="7170" width="15.44140625" customWidth="1"/>
+    <col min="7171" max="7171" width="40.109375" customWidth="1"/>
     <col min="7172" max="7172" width="22" customWidth="1"/>
-    <col min="7173" max="7173" width="25.7109375" customWidth="1"/>
-    <col min="7425" max="7425" width="9.140625" customWidth="1"/>
-    <col min="7426" max="7426" width="15.42578125" customWidth="1"/>
-    <col min="7427" max="7427" width="40.140625" customWidth="1"/>
+    <col min="7173" max="7173" width="25.6640625" customWidth="1"/>
+    <col min="7425" max="7425" width="9.109375" customWidth="1"/>
+    <col min="7426" max="7426" width="15.44140625" customWidth="1"/>
+    <col min="7427" max="7427" width="40.109375" customWidth="1"/>
     <col min="7428" max="7428" width="22" customWidth="1"/>
-    <col min="7429" max="7429" width="25.7109375" customWidth="1"/>
-    <col min="7681" max="7681" width="9.140625" customWidth="1"/>
-    <col min="7682" max="7682" width="15.42578125" customWidth="1"/>
-    <col min="7683" max="7683" width="40.140625" customWidth="1"/>
+    <col min="7429" max="7429" width="25.6640625" customWidth="1"/>
+    <col min="7681" max="7681" width="9.109375" customWidth="1"/>
+    <col min="7682" max="7682" width="15.44140625" customWidth="1"/>
+    <col min="7683" max="7683" width="40.109375" customWidth="1"/>
     <col min="7684" max="7684" width="22" customWidth="1"/>
-    <col min="7685" max="7685" width="25.7109375" customWidth="1"/>
-    <col min="7937" max="7937" width="9.140625" customWidth="1"/>
-    <col min="7938" max="7938" width="15.42578125" customWidth="1"/>
-    <col min="7939" max="7939" width="40.140625" customWidth="1"/>
+    <col min="7685" max="7685" width="25.6640625" customWidth="1"/>
+    <col min="7937" max="7937" width="9.109375" customWidth="1"/>
+    <col min="7938" max="7938" width="15.44140625" customWidth="1"/>
+    <col min="7939" max="7939" width="40.109375" customWidth="1"/>
     <col min="7940" max="7940" width="22" customWidth="1"/>
-    <col min="7941" max="7941" width="25.7109375" customWidth="1"/>
-    <col min="8193" max="8193" width="9.140625" customWidth="1"/>
-    <col min="8194" max="8194" width="15.42578125" customWidth="1"/>
-    <col min="8195" max="8195" width="40.140625" customWidth="1"/>
+    <col min="7941" max="7941" width="25.6640625" customWidth="1"/>
+    <col min="8193" max="8193" width="9.109375" customWidth="1"/>
+    <col min="8194" max="8194" width="15.44140625" customWidth="1"/>
+    <col min="8195" max="8195" width="40.109375" customWidth="1"/>
     <col min="8196" max="8196" width="22" customWidth="1"/>
-    <col min="8197" max="8197" width="25.7109375" customWidth="1"/>
-    <col min="8449" max="8449" width="9.140625" customWidth="1"/>
-    <col min="8450" max="8450" width="15.42578125" customWidth="1"/>
-    <col min="8451" max="8451" width="40.140625" customWidth="1"/>
+    <col min="8197" max="8197" width="25.6640625" customWidth="1"/>
+    <col min="8449" max="8449" width="9.109375" customWidth="1"/>
+    <col min="8450" max="8450" width="15.44140625" customWidth="1"/>
+    <col min="8451" max="8451" width="40.109375" customWidth="1"/>
     <col min="8452" max="8452" width="22" customWidth="1"/>
-    <col min="8453" max="8453" width="25.7109375" customWidth="1"/>
-    <col min="8705" max="8705" width="9.140625" customWidth="1"/>
-    <col min="8706" max="8706" width="15.42578125" customWidth="1"/>
-    <col min="8707" max="8707" width="40.140625" customWidth="1"/>
+    <col min="8453" max="8453" width="25.6640625" customWidth="1"/>
+    <col min="8705" max="8705" width="9.109375" customWidth="1"/>
+    <col min="8706" max="8706" width="15.44140625" customWidth="1"/>
+    <col min="8707" max="8707" width="40.109375" customWidth="1"/>
     <col min="8708" max="8708" width="22" customWidth="1"/>
-    <col min="8709" max="8709" width="25.7109375" customWidth="1"/>
-    <col min="8961" max="8961" width="9.140625" customWidth="1"/>
-    <col min="8962" max="8962" width="15.42578125" customWidth="1"/>
-    <col min="8963" max="8963" width="40.140625" customWidth="1"/>
+    <col min="8709" max="8709" width="25.6640625" customWidth="1"/>
+    <col min="8961" max="8961" width="9.109375" customWidth="1"/>
+    <col min="8962" max="8962" width="15.44140625" customWidth="1"/>
+    <col min="8963" max="8963" width="40.109375" customWidth="1"/>
     <col min="8964" max="8964" width="22" customWidth="1"/>
-    <col min="8965" max="8965" width="25.7109375" customWidth="1"/>
-    <col min="9217" max="9217" width="9.140625" customWidth="1"/>
-    <col min="9218" max="9218" width="15.42578125" customWidth="1"/>
-    <col min="9219" max="9219" width="40.140625" customWidth="1"/>
+    <col min="8965" max="8965" width="25.6640625" customWidth="1"/>
+    <col min="9217" max="9217" width="9.109375" customWidth="1"/>
+    <col min="9218" max="9218" width="15.44140625" customWidth="1"/>
+    <col min="9219" max="9219" width="40.109375" customWidth="1"/>
     <col min="9220" max="9220" width="22" customWidth="1"/>
-    <col min="9221" max="9221" width="25.7109375" customWidth="1"/>
-    <col min="9473" max="9473" width="9.140625" customWidth="1"/>
-    <col min="9474" max="9474" width="15.42578125" customWidth="1"/>
-    <col min="9475" max="9475" width="40.140625" customWidth="1"/>
+    <col min="9221" max="9221" width="25.6640625" customWidth="1"/>
+    <col min="9473" max="9473" width="9.109375" customWidth="1"/>
+    <col min="9474" max="9474" width="15.44140625" customWidth="1"/>
+    <col min="9475" max="9475" width="40.109375" customWidth="1"/>
     <col min="9476" max="9476" width="22" customWidth="1"/>
-    <col min="9477" max="9477" width="25.7109375" customWidth="1"/>
-    <col min="9729" max="9729" width="9.140625" customWidth="1"/>
-    <col min="9730" max="9730" width="15.42578125" customWidth="1"/>
-    <col min="9731" max="9731" width="40.140625" customWidth="1"/>
+    <col min="9477" max="9477" width="25.6640625" customWidth="1"/>
+    <col min="9729" max="9729" width="9.109375" customWidth="1"/>
+    <col min="9730" max="9730" width="15.44140625" customWidth="1"/>
+    <col min="9731" max="9731" width="40.109375" customWidth="1"/>
     <col min="9732" max="9732" width="22" customWidth="1"/>
-    <col min="9733" max="9733" width="25.7109375" customWidth="1"/>
-    <col min="9985" max="9985" width="9.140625" customWidth="1"/>
-    <col min="9986" max="9986" width="15.42578125" customWidth="1"/>
-    <col min="9987" max="9987" width="40.140625" customWidth="1"/>
+    <col min="9733" max="9733" width="25.6640625" customWidth="1"/>
+    <col min="9985" max="9985" width="9.109375" customWidth="1"/>
+    <col min="9986" max="9986" width="15.44140625" customWidth="1"/>
+    <col min="9987" max="9987" width="40.109375" customWidth="1"/>
     <col min="9988" max="9988" width="22" customWidth="1"/>
-    <col min="9989" max="9989" width="25.7109375" customWidth="1"/>
-    <col min="10241" max="10241" width="9.140625" customWidth="1"/>
-    <col min="10242" max="10242" width="15.42578125" customWidth="1"/>
-    <col min="10243" max="10243" width="40.140625" customWidth="1"/>
+    <col min="9989" max="9989" width="25.6640625" customWidth="1"/>
+    <col min="10241" max="10241" width="9.109375" customWidth="1"/>
+    <col min="10242" max="10242" width="15.44140625" customWidth="1"/>
+    <col min="10243" max="10243" width="40.109375" customWidth="1"/>
     <col min="10244" max="10244" width="22" customWidth="1"/>
-    <col min="10245" max="10245" width="25.7109375" customWidth="1"/>
-    <col min="10497" max="10497" width="9.140625" customWidth="1"/>
-    <col min="10498" max="10498" width="15.42578125" customWidth="1"/>
-    <col min="10499" max="10499" width="40.140625" customWidth="1"/>
+    <col min="10245" max="10245" width="25.6640625" customWidth="1"/>
+    <col min="10497" max="10497" width="9.109375" customWidth="1"/>
+    <col min="10498" max="10498" width="15.44140625" customWidth="1"/>
+    <col min="10499" max="10499" width="40.109375" customWidth="1"/>
     <col min="10500" max="10500" width="22" customWidth="1"/>
-    <col min="10501" max="10501" width="25.7109375" customWidth="1"/>
-    <col min="10753" max="10753" width="9.140625" customWidth="1"/>
-    <col min="10754" max="10754" width="15.42578125" customWidth="1"/>
-    <col min="10755" max="10755" width="40.140625" customWidth="1"/>
+    <col min="10501" max="10501" width="25.6640625" customWidth="1"/>
+    <col min="10753" max="10753" width="9.109375" customWidth="1"/>
+    <col min="10754" max="10754" width="15.44140625" customWidth="1"/>
+    <col min="10755" max="10755" width="40.109375" customWidth="1"/>
     <col min="10756" max="10756" width="22" customWidth="1"/>
-    <col min="10757" max="10757" width="25.7109375" customWidth="1"/>
-    <col min="11009" max="11009" width="9.140625" customWidth="1"/>
-    <col min="11010" max="11010" width="15.42578125" customWidth="1"/>
-    <col min="11011" max="11011" width="40.140625" customWidth="1"/>
+    <col min="10757" max="10757" width="25.6640625" customWidth="1"/>
+    <col min="11009" max="11009" width="9.109375" customWidth="1"/>
+    <col min="11010" max="11010" width="15.44140625" customWidth="1"/>
+    <col min="11011" max="11011" width="40.109375" customWidth="1"/>
     <col min="11012" max="11012" width="22" customWidth="1"/>
-    <col min="11013" max="11013" width="25.7109375" customWidth="1"/>
-    <col min="11265" max="11265" width="9.140625" customWidth="1"/>
-    <col min="11266" max="11266" width="15.42578125" customWidth="1"/>
-    <col min="11267" max="11267" width="40.140625" customWidth="1"/>
+    <col min="11013" max="11013" width="25.6640625" customWidth="1"/>
+    <col min="11265" max="11265" width="9.109375" customWidth="1"/>
+    <col min="11266" max="11266" width="15.44140625" customWidth="1"/>
+    <col min="11267" max="11267" width="40.109375" customWidth="1"/>
     <col min="11268" max="11268" width="22" customWidth="1"/>
-    <col min="11269" max="11269" width="25.7109375" customWidth="1"/>
-    <col min="11521" max="11521" width="9.140625" customWidth="1"/>
-    <col min="11522" max="11522" width="15.42578125" customWidth="1"/>
-    <col min="11523" max="11523" width="40.140625" customWidth="1"/>
+    <col min="11269" max="11269" width="25.6640625" customWidth="1"/>
+    <col min="11521" max="11521" width="9.109375" customWidth="1"/>
+    <col min="11522" max="11522" width="15.44140625" customWidth="1"/>
+    <col min="11523" max="11523" width="40.109375" customWidth="1"/>
     <col min="11524" max="11524" width="22" customWidth="1"/>
-    <col min="11525" max="11525" width="25.7109375" customWidth="1"/>
-    <col min="11777" max="11777" width="9.140625" customWidth="1"/>
-    <col min="11778" max="11778" width="15.42578125" customWidth="1"/>
-    <col min="11779" max="11779" width="40.140625" customWidth="1"/>
+    <col min="11525" max="11525" width="25.6640625" customWidth="1"/>
+    <col min="11777" max="11777" width="9.109375" customWidth="1"/>
+    <col min="11778" max="11778" width="15.44140625" customWidth="1"/>
+    <col min="11779" max="11779" width="40.109375" customWidth="1"/>
     <col min="11780" max="11780" width="22" customWidth="1"/>
-    <col min="11781" max="11781" width="25.7109375" customWidth="1"/>
-    <col min="12033" max="12033" width="9.140625" customWidth="1"/>
-    <col min="12034" max="12034" width="15.42578125" customWidth="1"/>
-    <col min="12035" max="12035" width="40.140625" customWidth="1"/>
+    <col min="11781" max="11781" width="25.6640625" customWidth="1"/>
+    <col min="12033" max="12033" width="9.109375" customWidth="1"/>
+    <col min="12034" max="12034" width="15.44140625" customWidth="1"/>
+    <col min="12035" max="12035" width="40.109375" customWidth="1"/>
     <col min="12036" max="12036" width="22" customWidth="1"/>
-    <col min="12037" max="12037" width="25.7109375" customWidth="1"/>
-    <col min="12289" max="12289" width="9.140625" customWidth="1"/>
-    <col min="12290" max="12290" width="15.42578125" customWidth="1"/>
-    <col min="12291" max="12291" width="40.140625" customWidth="1"/>
+    <col min="12037" max="12037" width="25.6640625" customWidth="1"/>
+    <col min="12289" max="12289" width="9.109375" customWidth="1"/>
+    <col min="12290" max="12290" width="15.44140625" customWidth="1"/>
+    <col min="12291" max="12291" width="40.109375" customWidth="1"/>
     <col min="12292" max="12292" width="22" customWidth="1"/>
-    <col min="12293" max="12293" width="25.7109375" customWidth="1"/>
-    <col min="12545" max="12545" width="9.140625" customWidth="1"/>
-    <col min="12546" max="12546" width="15.42578125" customWidth="1"/>
-    <col min="12547" max="12547" width="40.140625" customWidth="1"/>
+    <col min="12293" max="12293" width="25.6640625" customWidth="1"/>
+    <col min="12545" max="12545" width="9.109375" customWidth="1"/>
+    <col min="12546" max="12546" width="15.44140625" customWidth="1"/>
+    <col min="12547" max="12547" width="40.109375" customWidth="1"/>
     <col min="12548" max="12548" width="22" customWidth="1"/>
-    <col min="12549" max="12549" width="25.7109375" customWidth="1"/>
-    <col min="12801" max="12801" width="9.140625" customWidth="1"/>
-    <col min="12802" max="12802" width="15.42578125" customWidth="1"/>
-    <col min="12803" max="12803" width="40.140625" customWidth="1"/>
+    <col min="12549" max="12549" width="25.6640625" customWidth="1"/>
+    <col min="12801" max="12801" width="9.109375" customWidth="1"/>
+    <col min="12802" max="12802" width="15.44140625" customWidth="1"/>
+    <col min="12803" max="12803" width="40.109375" customWidth="1"/>
     <col min="12804" max="12804" width="22" customWidth="1"/>
-    <col min="12805" max="12805" width="25.7109375" customWidth="1"/>
-    <col min="13057" max="13057" width="9.140625" customWidth="1"/>
-    <col min="13058" max="13058" width="15.42578125" customWidth="1"/>
-    <col min="13059" max="13059" width="40.140625" customWidth="1"/>
+    <col min="12805" max="12805" width="25.6640625" customWidth="1"/>
+    <col min="13057" max="13057" width="9.109375" customWidth="1"/>
+    <col min="13058" max="13058" width="15.44140625" customWidth="1"/>
+    <col min="13059" max="13059" width="40.109375" customWidth="1"/>
     <col min="13060" max="13060" width="22" customWidth="1"/>
-    <col min="13061" max="13061" width="25.7109375" customWidth="1"/>
-    <col min="13313" max="13313" width="9.140625" customWidth="1"/>
-    <col min="13314" max="13314" width="15.42578125" customWidth="1"/>
-    <col min="13315" max="13315" width="40.140625" customWidth="1"/>
+    <col min="13061" max="13061" width="25.6640625" customWidth="1"/>
+    <col min="13313" max="13313" width="9.109375" customWidth="1"/>
+    <col min="13314" max="13314" width="15.44140625" customWidth="1"/>
+    <col min="13315" max="13315" width="40.109375" customWidth="1"/>
     <col min="13316" max="13316" width="22" customWidth="1"/>
-    <col min="13317" max="13317" width="25.7109375" customWidth="1"/>
-    <col min="13569" max="13569" width="9.140625" customWidth="1"/>
-    <col min="13570" max="13570" width="15.42578125" customWidth="1"/>
-    <col min="13571" max="13571" width="40.140625" customWidth="1"/>
+    <col min="13317" max="13317" width="25.6640625" customWidth="1"/>
+    <col min="13569" max="13569" width="9.109375" customWidth="1"/>
+    <col min="13570" max="13570" width="15.44140625" customWidth="1"/>
+    <col min="13571" max="13571" width="40.109375" customWidth="1"/>
     <col min="13572" max="13572" width="22" customWidth="1"/>
-    <col min="13573" max="13573" width="25.7109375" customWidth="1"/>
-    <col min="13825" max="13825" width="9.140625" customWidth="1"/>
-    <col min="13826" max="13826" width="15.42578125" customWidth="1"/>
-    <col min="13827" max="13827" width="40.140625" customWidth="1"/>
+    <col min="13573" max="13573" width="25.6640625" customWidth="1"/>
+    <col min="13825" max="13825" width="9.109375" customWidth="1"/>
+    <col min="13826" max="13826" width="15.44140625" customWidth="1"/>
+    <col min="13827" max="13827" width="40.109375" customWidth="1"/>
     <col min="13828" max="13828" width="22" customWidth="1"/>
-    <col min="13829" max="13829" width="25.7109375" customWidth="1"/>
-    <col min="14081" max="14081" width="9.140625" customWidth="1"/>
-    <col min="14082" max="14082" width="15.42578125" customWidth="1"/>
-    <col min="14083" max="14083" width="40.140625" customWidth="1"/>
+    <col min="13829" max="13829" width="25.6640625" customWidth="1"/>
+    <col min="14081" max="14081" width="9.109375" customWidth="1"/>
+    <col min="14082" max="14082" width="15.44140625" customWidth="1"/>
+    <col min="14083" max="14083" width="40.109375" customWidth="1"/>
     <col min="14084" max="14084" width="22" customWidth="1"/>
-    <col min="14085" max="14085" width="25.7109375" customWidth="1"/>
-    <col min="14337" max="14337" width="9.140625" customWidth="1"/>
-    <col min="14338" max="14338" width="15.42578125" customWidth="1"/>
-    <col min="14339" max="14339" width="40.140625" customWidth="1"/>
+    <col min="14085" max="14085" width="25.6640625" customWidth="1"/>
+    <col min="14337" max="14337" width="9.109375" customWidth="1"/>
+    <col min="14338" max="14338" width="15.44140625" customWidth="1"/>
+    <col min="14339" max="14339" width="40.109375" customWidth="1"/>
     <col min="14340" max="14340" width="22" customWidth="1"/>
-    <col min="14341" max="14341" width="25.7109375" customWidth="1"/>
-    <col min="14593" max="14593" width="9.140625" customWidth="1"/>
-    <col min="14594" max="14594" width="15.42578125" customWidth="1"/>
-    <col min="14595" max="14595" width="40.140625" customWidth="1"/>
+    <col min="14341" max="14341" width="25.6640625" customWidth="1"/>
+    <col min="14593" max="14593" width="9.109375" customWidth="1"/>
+    <col min="14594" max="14594" width="15.44140625" customWidth="1"/>
+    <col min="14595" max="14595" width="40.109375" customWidth="1"/>
     <col min="14596" max="14596" width="22" customWidth="1"/>
-    <col min="14597" max="14597" width="25.7109375" customWidth="1"/>
-    <col min="14849" max="14849" width="9.140625" customWidth="1"/>
-    <col min="14850" max="14850" width="15.42578125" customWidth="1"/>
-    <col min="14851" max="14851" width="40.140625" customWidth="1"/>
+    <col min="14597" max="14597" width="25.6640625" customWidth="1"/>
+    <col min="14849" max="14849" width="9.109375" customWidth="1"/>
+    <col min="14850" max="14850" width="15.44140625" customWidth="1"/>
+    <col min="14851" max="14851" width="40.109375" customWidth="1"/>
     <col min="14852" max="14852" width="22" customWidth="1"/>
-    <col min="14853" max="14853" width="25.7109375" customWidth="1"/>
-    <col min="15105" max="15105" width="9.140625" customWidth="1"/>
-    <col min="15106" max="15106" width="15.42578125" customWidth="1"/>
-    <col min="15107" max="15107" width="40.140625" customWidth="1"/>
+    <col min="14853" max="14853" width="25.6640625" customWidth="1"/>
+    <col min="15105" max="15105" width="9.109375" customWidth="1"/>
+    <col min="15106" max="15106" width="15.44140625" customWidth="1"/>
+    <col min="15107" max="15107" width="40.109375" customWidth="1"/>
     <col min="15108" max="15108" width="22" customWidth="1"/>
-    <col min="15109" max="15109" width="25.7109375" customWidth="1"/>
-    <col min="15361" max="15361" width="9.140625" customWidth="1"/>
-    <col min="15362" max="15362" width="15.42578125" customWidth="1"/>
-    <col min="15363" max="15363" width="40.140625" customWidth="1"/>
+    <col min="15109" max="15109" width="25.6640625" customWidth="1"/>
+    <col min="15361" max="15361" width="9.109375" customWidth="1"/>
+    <col min="15362" max="15362" width="15.44140625" customWidth="1"/>
+    <col min="15363" max="15363" width="40.109375" customWidth="1"/>
     <col min="15364" max="15364" width="22" customWidth="1"/>
-    <col min="15365" max="15365" width="25.7109375" customWidth="1"/>
-    <col min="15617" max="15617" width="9.140625" customWidth="1"/>
-    <col min="15618" max="15618" width="15.42578125" customWidth="1"/>
-    <col min="15619" max="15619" width="40.140625" customWidth="1"/>
+    <col min="15365" max="15365" width="25.6640625" customWidth="1"/>
+    <col min="15617" max="15617" width="9.109375" customWidth="1"/>
+    <col min="15618" max="15618" width="15.44140625" customWidth="1"/>
+    <col min="15619" max="15619" width="40.109375" customWidth="1"/>
     <col min="15620" max="15620" width="22" customWidth="1"/>
-    <col min="15621" max="15621" width="25.7109375" customWidth="1"/>
-    <col min="15873" max="15873" width="9.140625" customWidth="1"/>
-    <col min="15874" max="15874" width="15.42578125" customWidth="1"/>
-    <col min="15875" max="15875" width="40.140625" customWidth="1"/>
+    <col min="15621" max="15621" width="25.6640625" customWidth="1"/>
+    <col min="15873" max="15873" width="9.109375" customWidth="1"/>
+    <col min="15874" max="15874" width="15.44140625" customWidth="1"/>
+    <col min="15875" max="15875" width="40.109375" customWidth="1"/>
     <col min="15876" max="15876" width="22" customWidth="1"/>
-    <col min="15877" max="15877" width="25.7109375" customWidth="1"/>
-    <col min="16129" max="16129" width="9.140625" customWidth="1"/>
-    <col min="16130" max="16130" width="15.42578125" customWidth="1"/>
-    <col min="16131" max="16131" width="40.140625" customWidth="1"/>
+    <col min="15877" max="15877" width="25.6640625" customWidth="1"/>
+    <col min="16129" max="16129" width="9.109375" customWidth="1"/>
+    <col min="16130" max="16130" width="15.44140625" customWidth="1"/>
+    <col min="16131" max="16131" width="40.109375" customWidth="1"/>
     <col min="16132" max="16132" width="22" customWidth="1"/>
-    <col min="16133" max="16133" width="25.7109375" customWidth="1"/>
+    <col min="16133" max="16133" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>23</v>
       </c>
@@ -876,7 +924,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="6">
         <v>42255</v>
       </c>
@@ -890,7 +938,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="26.4" x14ac:dyDescent="0.3">
       <c r="B6" s="6">
         <v>42451</v>
       </c>
@@ -904,295 +952,303 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B7" s="6">
+        <v>43122</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1.02</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="6"/>
       <c r="C8" s="9"/>
       <c r="D8" s="11"/>
       <c r="E8" s="10"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
       <c r="C9" s="9"/>
       <c r="D9" s="11"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="11"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
       <c r="D11" s="11"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
       <c r="C12" s="9"/>
       <c r="D12" s="11"/>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="11"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="11"/>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="9"/>
       <c r="D15" s="11"/>
       <c r="E15" s="10"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
       <c r="D16" s="11"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
       <c r="D17" s="11"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
       <c r="D18" s="11"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="11"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="11"/>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
       <c r="D21" s="11"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="6"/>
       <c r="C22" s="9"/>
       <c r="D22" s="11"/>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="11"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
       <c r="D24" s="11"/>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="11"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="6"/>
       <c r="C26" s="9"/>
       <c r="D26" s="11"/>
       <c r="E26" s="10"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="11"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="12"/>
       <c r="C28" s="7"/>
       <c r="D28" s="11"/>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="12"/>
       <c r="C29" s="9"/>
       <c r="D29" s="11"/>
       <c r="E29" s="10"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="12"/>
       <c r="C30" s="9"/>
       <c r="D30" s="11"/>
       <c r="E30" s="10"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
       <c r="D31" s="11"/>
       <c r="E31" s="10"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" s="12"/>
       <c r="D32" s="11"/>
       <c r="E32" s="10"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="12"/>
       <c r="D33" s="11"/>
       <c r="E33" s="10"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="12"/>
       <c r="C34" s="13"/>
       <c r="D34" s="11"/>
       <c r="E34" s="10"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="12"/>
       <c r="D35" s="11"/>
       <c r="E35" s="10"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="12"/>
       <c r="D36" s="11"/>
       <c r="E36" s="10"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="12"/>
       <c r="D37" s="11"/>
       <c r="E37" s="10"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="12"/>
       <c r="D38" s="11"/>
       <c r="E38" s="10"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="12"/>
       <c r="D39" s="11"/>
       <c r="E39" s="10"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="12"/>
       <c r="D40" s="11"/>
       <c r="E40" s="10"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="12"/>
       <c r="C41" s="13"/>
       <c r="D41" s="11"/>
       <c r="E41" s="10"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="12"/>
       <c r="C42" s="13"/>
       <c r="D42" s="11"/>
       <c r="E42" s="10"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="12"/>
       <c r="D43" s="11"/>
       <c r="E43" s="10"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" s="12"/>
       <c r="D44" s="11"/>
       <c r="E44" s="10"/>
     </row>
-    <row r="45" spans="2:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="12"/>
       <c r="D45" s="11"/>
       <c r="E45" s="10"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="12"/>
       <c r="D46" s="11"/>
       <c r="E46" s="10"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="12"/>
       <c r="D47" s="11"/>
       <c r="E47" s="10"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="12"/>
       <c r="D48" s="11"/>
       <c r="E48" s="10"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="12"/>
       <c r="D49" s="11"/>
       <c r="E49" s="10"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="12"/>
       <c r="D50" s="11"/>
       <c r="E50" s="10"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" s="12"/>
       <c r="D51" s="11"/>
       <c r="E51" s="10"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="12"/>
       <c r="D52" s="11"/>
       <c r="E52" s="10"/>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="12"/>
       <c r="D53" s="11"/>
       <c r="E53" s="10"/>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="12"/>
       <c r="D54" s="11"/>
       <c r="E54" s="10"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B55" s="12"/>
       <c r="D55" s="11"/>
       <c r="E55" s="10"/>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B56" s="12"/>
       <c r="D56" s="11"/>
       <c r="E56" s="10"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B57" s="12"/>
       <c r="D57" s="11"/>
       <c r="E57" s="10"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58" s="12"/>
       <c r="D58" s="11"/>
       <c r="E58" s="10"/>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B59" s="12"/>
       <c r="D59" s="11"/>
       <c r="E59" s="10"/>
@@ -1205,229 +1261,367 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="12">
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="12">
         <v>42255</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="12">
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="12">
         <v>42255</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="12">
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="12">
         <v>42255</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="2">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="12">
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="12">
         <v>42255</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="2">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="12">
+      <c r="I6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="12">
         <v>42255</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>5</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="12">
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="12">
         <v>42255</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
         <v>5</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
         <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" s="15">
+        <v>43150</v>
       </c>
     </row>
   </sheetData>
@@ -1442,7 +1636,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tfs9511 - ecl survey pilot
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C39457
</commit_message>
<xml_diff>
--- a/Requirements/CCO_eCoaching_Log_Survey_Questions.xlsx
+++ b/Requirements/CCO_eCoaching_Log_Survey_Questions.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="48">
   <si>
     <t>Survey Question</t>
   </si>
@@ -134,13 +134,6 @@
   </si>
   <si>
     <t>How prepared was your supervisor during your coaching session?</t>
-  </si>
-  <si>
-    <t>1 - Very Prepared
-2 - Prepared
-3 - Neither Prepared or Unprepared
-4 - Unprepared
-5 - Very Unprepared</t>
   </si>
   <si>
     <t>Site</t>
@@ -183,6 +176,16 @@
 Quality
 Recognition
 Secure Floor Violations</t>
+  </si>
+  <si>
+    <t>1 - Very Unprepared
+2 - Unprepared
+3 - Neither Prepared or Unprepared
+4 - Prepared
+5 - Very Prepared</t>
+  </si>
+  <si>
+    <t>TFS6511 - eCL Pilot Survey Question - changed order of responses and added follow up on line 7</t>
   </si>
 </sst>
 </file>
@@ -587,7 +590,7 @@
   <dimension ref="B4:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -961,7 +964,7 @@
         <v>43122</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="11">
         <v>1.02</v>
@@ -975,7 +978,7 @@
         <v>43123</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="11">
         <v>1.03</v>
@@ -984,11 +987,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="6"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="8"/>
+    <row r="9" spans="2:5" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="6">
+        <v>43129</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1.04</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
@@ -1276,7 +1287,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1299,10 +1310,10 @@
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>0</v>
@@ -1320,13 +1331,13 @@
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>29</v>
@@ -1340,7 +1351,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1361,7 +1372,7 @@
         <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
@@ -1378,7 +1389,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -1399,7 +1410,7 @@
         <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
@@ -1416,7 +1427,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -1437,7 +1448,7 @@
         <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J4" t="s">
         <v>18</v>
@@ -1454,7 +1465,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -1475,7 +1486,7 @@
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J5" t="s">
         <v>18</v>
@@ -1492,7 +1503,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
@@ -1513,7 +1524,7 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J6" t="s">
         <v>18</v>
@@ -1530,7 +1541,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="2">
         <v>6</v>
@@ -1542,16 +1553,16 @@
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>18</v>
@@ -1603,7 +1614,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2">
         <v>99</v>
@@ -1624,7 +1635,7 @@
         <v>4</v>
       </c>
       <c r="I9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J9" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
tfs10890 - ecl disable pilot survey
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C39979
</commit_message>
<xml_diff>
--- a/Requirements/CCO_eCoaching_Log_Survey_Questions.xlsx
+++ b/Requirements/CCO_eCoaching_Log_Survey_Questions.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="49">
   <si>
     <t>Survey Question</t>
   </si>
@@ -186,6 +186,10 @@
   </si>
   <si>
     <t>TFS6511 - eCL Pilot Survey Question - changed order of responses and added follow up on line 7</t>
+  </si>
+  <si>
+    <t>tfs10890 - ecl disable pilot survey question
+set active to No and end date to 05/04/2018</t>
   </si>
 </sst>
 </file>
@@ -590,7 +594,7 @@
   <dimension ref="B4:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1001,11 +1005,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="8"/>
+    <row r="10" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="6">
+        <v>43224</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="11">
+        <v>1.05</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="6"/>
@@ -1287,7 +1299,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1538,7 +1550,7 @@
     </row>
     <row r="7" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>37</v>
@@ -1572,6 +1584,9 @@
       </c>
       <c r="L7" s="15">
         <v>43150</v>
+      </c>
+      <c r="M7" s="12">
+        <v>43224</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
TFS14209 Added new Hot Topic Pilot question
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C42212
</commit_message>
<xml_diff>
--- a/Requirements/CCO_eCoaching_Log_Survey_Questions.xlsx
+++ b/Requirements/CCO_eCoaching_Log_Survey_Questions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian.coughlin\Documents\TFS\OY6\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="72" windowWidth="18192" windowHeight="11820" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="54">
   <si>
     <t>Survey Question</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>Hot Topic</t>
   </si>
   <si>
     <t>1 - Very Ineffective
@@ -191,11 +188,35 @@
     <t>tfs10890 - ecl disable pilot survey question
 set active to No and end date to 05/04/2018</t>
   </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Quality Now has improved my experience working on the CCO</t>
+  </si>
+  <si>
+    <t>1 - Strongly Disagree
+2 - Disagree
+3 - Somewhat Disagree
+4 - Neutral
+5 - Somewhat Agree
+6 - Agree
+7 - Strongly Agree</t>
+  </si>
+  <si>
+    <t>Verint CCO or Verint CCO Supervisor</t>
+  </si>
+  <si>
+    <t>Brian Coughlin</t>
+  </si>
+  <si>
+    <t>TFS14209 - eCoaching - Add new Hot Topic Survey question 5/1-7/1/2019</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -594,696 +615,704 @@
   <dimension ref="B4:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="40.109375" style="14" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" style="14" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
-    <col min="257" max="257" width="9.109375" customWidth="1"/>
-    <col min="258" max="258" width="15.44140625" customWidth="1"/>
-    <col min="259" max="259" width="40.109375" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="257" max="257" width="9.140625" customWidth="1"/>
+    <col min="258" max="258" width="15.42578125" customWidth="1"/>
+    <col min="259" max="259" width="40.140625" customWidth="1"/>
     <col min="260" max="260" width="22" customWidth="1"/>
-    <col min="261" max="261" width="25.6640625" customWidth="1"/>
-    <col min="513" max="513" width="9.109375" customWidth="1"/>
-    <col min="514" max="514" width="15.44140625" customWidth="1"/>
-    <col min="515" max="515" width="40.109375" customWidth="1"/>
+    <col min="261" max="261" width="25.7109375" customWidth="1"/>
+    <col min="513" max="513" width="9.140625" customWidth="1"/>
+    <col min="514" max="514" width="15.42578125" customWidth="1"/>
+    <col min="515" max="515" width="40.140625" customWidth="1"/>
     <col min="516" max="516" width="22" customWidth="1"/>
-    <col min="517" max="517" width="25.6640625" customWidth="1"/>
-    <col min="769" max="769" width="9.109375" customWidth="1"/>
-    <col min="770" max="770" width="15.44140625" customWidth="1"/>
-    <col min="771" max="771" width="40.109375" customWidth="1"/>
+    <col min="517" max="517" width="25.7109375" customWidth="1"/>
+    <col min="769" max="769" width="9.140625" customWidth="1"/>
+    <col min="770" max="770" width="15.42578125" customWidth="1"/>
+    <col min="771" max="771" width="40.140625" customWidth="1"/>
     <col min="772" max="772" width="22" customWidth="1"/>
-    <col min="773" max="773" width="25.6640625" customWidth="1"/>
-    <col min="1025" max="1025" width="9.109375" customWidth="1"/>
-    <col min="1026" max="1026" width="15.44140625" customWidth="1"/>
-    <col min="1027" max="1027" width="40.109375" customWidth="1"/>
+    <col min="773" max="773" width="25.7109375" customWidth="1"/>
+    <col min="1025" max="1025" width="9.140625" customWidth="1"/>
+    <col min="1026" max="1026" width="15.42578125" customWidth="1"/>
+    <col min="1027" max="1027" width="40.140625" customWidth="1"/>
     <col min="1028" max="1028" width="22" customWidth="1"/>
-    <col min="1029" max="1029" width="25.6640625" customWidth="1"/>
-    <col min="1281" max="1281" width="9.109375" customWidth="1"/>
-    <col min="1282" max="1282" width="15.44140625" customWidth="1"/>
-    <col min="1283" max="1283" width="40.109375" customWidth="1"/>
+    <col min="1029" max="1029" width="25.7109375" customWidth="1"/>
+    <col min="1281" max="1281" width="9.140625" customWidth="1"/>
+    <col min="1282" max="1282" width="15.42578125" customWidth="1"/>
+    <col min="1283" max="1283" width="40.140625" customWidth="1"/>
     <col min="1284" max="1284" width="22" customWidth="1"/>
-    <col min="1285" max="1285" width="25.6640625" customWidth="1"/>
-    <col min="1537" max="1537" width="9.109375" customWidth="1"/>
-    <col min="1538" max="1538" width="15.44140625" customWidth="1"/>
-    <col min="1539" max="1539" width="40.109375" customWidth="1"/>
+    <col min="1285" max="1285" width="25.7109375" customWidth="1"/>
+    <col min="1537" max="1537" width="9.140625" customWidth="1"/>
+    <col min="1538" max="1538" width="15.42578125" customWidth="1"/>
+    <col min="1539" max="1539" width="40.140625" customWidth="1"/>
     <col min="1540" max="1540" width="22" customWidth="1"/>
-    <col min="1541" max="1541" width="25.6640625" customWidth="1"/>
-    <col min="1793" max="1793" width="9.109375" customWidth="1"/>
-    <col min="1794" max="1794" width="15.44140625" customWidth="1"/>
-    <col min="1795" max="1795" width="40.109375" customWidth="1"/>
+    <col min="1541" max="1541" width="25.7109375" customWidth="1"/>
+    <col min="1793" max="1793" width="9.140625" customWidth="1"/>
+    <col min="1794" max="1794" width="15.42578125" customWidth="1"/>
+    <col min="1795" max="1795" width="40.140625" customWidth="1"/>
     <col min="1796" max="1796" width="22" customWidth="1"/>
-    <col min="1797" max="1797" width="25.6640625" customWidth="1"/>
-    <col min="2049" max="2049" width="9.109375" customWidth="1"/>
-    <col min="2050" max="2050" width="15.44140625" customWidth="1"/>
-    <col min="2051" max="2051" width="40.109375" customWidth="1"/>
+    <col min="1797" max="1797" width="25.7109375" customWidth="1"/>
+    <col min="2049" max="2049" width="9.140625" customWidth="1"/>
+    <col min="2050" max="2050" width="15.42578125" customWidth="1"/>
+    <col min="2051" max="2051" width="40.140625" customWidth="1"/>
     <col min="2052" max="2052" width="22" customWidth="1"/>
-    <col min="2053" max="2053" width="25.6640625" customWidth="1"/>
-    <col min="2305" max="2305" width="9.109375" customWidth="1"/>
-    <col min="2306" max="2306" width="15.44140625" customWidth="1"/>
-    <col min="2307" max="2307" width="40.109375" customWidth="1"/>
+    <col min="2053" max="2053" width="25.7109375" customWidth="1"/>
+    <col min="2305" max="2305" width="9.140625" customWidth="1"/>
+    <col min="2306" max="2306" width="15.42578125" customWidth="1"/>
+    <col min="2307" max="2307" width="40.140625" customWidth="1"/>
     <col min="2308" max="2308" width="22" customWidth="1"/>
-    <col min="2309" max="2309" width="25.6640625" customWidth="1"/>
-    <col min="2561" max="2561" width="9.109375" customWidth="1"/>
-    <col min="2562" max="2562" width="15.44140625" customWidth="1"/>
-    <col min="2563" max="2563" width="40.109375" customWidth="1"/>
+    <col min="2309" max="2309" width="25.7109375" customWidth="1"/>
+    <col min="2561" max="2561" width="9.140625" customWidth="1"/>
+    <col min="2562" max="2562" width="15.42578125" customWidth="1"/>
+    <col min="2563" max="2563" width="40.140625" customWidth="1"/>
     <col min="2564" max="2564" width="22" customWidth="1"/>
-    <col min="2565" max="2565" width="25.6640625" customWidth="1"/>
-    <col min="2817" max="2817" width="9.109375" customWidth="1"/>
-    <col min="2818" max="2818" width="15.44140625" customWidth="1"/>
-    <col min="2819" max="2819" width="40.109375" customWidth="1"/>
+    <col min="2565" max="2565" width="25.7109375" customWidth="1"/>
+    <col min="2817" max="2817" width="9.140625" customWidth="1"/>
+    <col min="2818" max="2818" width="15.42578125" customWidth="1"/>
+    <col min="2819" max="2819" width="40.140625" customWidth="1"/>
     <col min="2820" max="2820" width="22" customWidth="1"/>
-    <col min="2821" max="2821" width="25.6640625" customWidth="1"/>
-    <col min="3073" max="3073" width="9.109375" customWidth="1"/>
-    <col min="3074" max="3074" width="15.44140625" customWidth="1"/>
-    <col min="3075" max="3075" width="40.109375" customWidth="1"/>
+    <col min="2821" max="2821" width="25.7109375" customWidth="1"/>
+    <col min="3073" max="3073" width="9.140625" customWidth="1"/>
+    <col min="3074" max="3074" width="15.42578125" customWidth="1"/>
+    <col min="3075" max="3075" width="40.140625" customWidth="1"/>
     <col min="3076" max="3076" width="22" customWidth="1"/>
-    <col min="3077" max="3077" width="25.6640625" customWidth="1"/>
-    <col min="3329" max="3329" width="9.109375" customWidth="1"/>
-    <col min="3330" max="3330" width="15.44140625" customWidth="1"/>
-    <col min="3331" max="3331" width="40.109375" customWidth="1"/>
+    <col min="3077" max="3077" width="25.7109375" customWidth="1"/>
+    <col min="3329" max="3329" width="9.140625" customWidth="1"/>
+    <col min="3330" max="3330" width="15.42578125" customWidth="1"/>
+    <col min="3331" max="3331" width="40.140625" customWidth="1"/>
     <col min="3332" max="3332" width="22" customWidth="1"/>
-    <col min="3333" max="3333" width="25.6640625" customWidth="1"/>
-    <col min="3585" max="3585" width="9.109375" customWidth="1"/>
-    <col min="3586" max="3586" width="15.44140625" customWidth="1"/>
-    <col min="3587" max="3587" width="40.109375" customWidth="1"/>
+    <col min="3333" max="3333" width="25.7109375" customWidth="1"/>
+    <col min="3585" max="3585" width="9.140625" customWidth="1"/>
+    <col min="3586" max="3586" width="15.42578125" customWidth="1"/>
+    <col min="3587" max="3587" width="40.140625" customWidth="1"/>
     <col min="3588" max="3588" width="22" customWidth="1"/>
-    <col min="3589" max="3589" width="25.6640625" customWidth="1"/>
-    <col min="3841" max="3841" width="9.109375" customWidth="1"/>
-    <col min="3842" max="3842" width="15.44140625" customWidth="1"/>
-    <col min="3843" max="3843" width="40.109375" customWidth="1"/>
+    <col min="3589" max="3589" width="25.7109375" customWidth="1"/>
+    <col min="3841" max="3841" width="9.140625" customWidth="1"/>
+    <col min="3842" max="3842" width="15.42578125" customWidth="1"/>
+    <col min="3843" max="3843" width="40.140625" customWidth="1"/>
     <col min="3844" max="3844" width="22" customWidth="1"/>
-    <col min="3845" max="3845" width="25.6640625" customWidth="1"/>
-    <col min="4097" max="4097" width="9.109375" customWidth="1"/>
-    <col min="4098" max="4098" width="15.44140625" customWidth="1"/>
-    <col min="4099" max="4099" width="40.109375" customWidth="1"/>
+    <col min="3845" max="3845" width="25.7109375" customWidth="1"/>
+    <col min="4097" max="4097" width="9.140625" customWidth="1"/>
+    <col min="4098" max="4098" width="15.42578125" customWidth="1"/>
+    <col min="4099" max="4099" width="40.140625" customWidth="1"/>
     <col min="4100" max="4100" width="22" customWidth="1"/>
-    <col min="4101" max="4101" width="25.6640625" customWidth="1"/>
-    <col min="4353" max="4353" width="9.109375" customWidth="1"/>
-    <col min="4354" max="4354" width="15.44140625" customWidth="1"/>
-    <col min="4355" max="4355" width="40.109375" customWidth="1"/>
+    <col min="4101" max="4101" width="25.7109375" customWidth="1"/>
+    <col min="4353" max="4353" width="9.140625" customWidth="1"/>
+    <col min="4354" max="4354" width="15.42578125" customWidth="1"/>
+    <col min="4355" max="4355" width="40.140625" customWidth="1"/>
     <col min="4356" max="4356" width="22" customWidth="1"/>
-    <col min="4357" max="4357" width="25.6640625" customWidth="1"/>
-    <col min="4609" max="4609" width="9.109375" customWidth="1"/>
-    <col min="4610" max="4610" width="15.44140625" customWidth="1"/>
-    <col min="4611" max="4611" width="40.109375" customWidth="1"/>
+    <col min="4357" max="4357" width="25.7109375" customWidth="1"/>
+    <col min="4609" max="4609" width="9.140625" customWidth="1"/>
+    <col min="4610" max="4610" width="15.42578125" customWidth="1"/>
+    <col min="4611" max="4611" width="40.140625" customWidth="1"/>
     <col min="4612" max="4612" width="22" customWidth="1"/>
-    <col min="4613" max="4613" width="25.6640625" customWidth="1"/>
-    <col min="4865" max="4865" width="9.109375" customWidth="1"/>
-    <col min="4866" max="4866" width="15.44140625" customWidth="1"/>
-    <col min="4867" max="4867" width="40.109375" customWidth="1"/>
+    <col min="4613" max="4613" width="25.7109375" customWidth="1"/>
+    <col min="4865" max="4865" width="9.140625" customWidth="1"/>
+    <col min="4866" max="4866" width="15.42578125" customWidth="1"/>
+    <col min="4867" max="4867" width="40.140625" customWidth="1"/>
     <col min="4868" max="4868" width="22" customWidth="1"/>
-    <col min="4869" max="4869" width="25.6640625" customWidth="1"/>
-    <col min="5121" max="5121" width="9.109375" customWidth="1"/>
-    <col min="5122" max="5122" width="15.44140625" customWidth="1"/>
-    <col min="5123" max="5123" width="40.109375" customWidth="1"/>
+    <col min="4869" max="4869" width="25.7109375" customWidth="1"/>
+    <col min="5121" max="5121" width="9.140625" customWidth="1"/>
+    <col min="5122" max="5122" width="15.42578125" customWidth="1"/>
+    <col min="5123" max="5123" width="40.140625" customWidth="1"/>
     <col min="5124" max="5124" width="22" customWidth="1"/>
-    <col min="5125" max="5125" width="25.6640625" customWidth="1"/>
-    <col min="5377" max="5377" width="9.109375" customWidth="1"/>
-    <col min="5378" max="5378" width="15.44140625" customWidth="1"/>
-    <col min="5379" max="5379" width="40.109375" customWidth="1"/>
+    <col min="5125" max="5125" width="25.7109375" customWidth="1"/>
+    <col min="5377" max="5377" width="9.140625" customWidth="1"/>
+    <col min="5378" max="5378" width="15.42578125" customWidth="1"/>
+    <col min="5379" max="5379" width="40.140625" customWidth="1"/>
     <col min="5380" max="5380" width="22" customWidth="1"/>
-    <col min="5381" max="5381" width="25.6640625" customWidth="1"/>
-    <col min="5633" max="5633" width="9.109375" customWidth="1"/>
-    <col min="5634" max="5634" width="15.44140625" customWidth="1"/>
-    <col min="5635" max="5635" width="40.109375" customWidth="1"/>
+    <col min="5381" max="5381" width="25.7109375" customWidth="1"/>
+    <col min="5633" max="5633" width="9.140625" customWidth="1"/>
+    <col min="5634" max="5634" width="15.42578125" customWidth="1"/>
+    <col min="5635" max="5635" width="40.140625" customWidth="1"/>
     <col min="5636" max="5636" width="22" customWidth="1"/>
-    <col min="5637" max="5637" width="25.6640625" customWidth="1"/>
-    <col min="5889" max="5889" width="9.109375" customWidth="1"/>
-    <col min="5890" max="5890" width="15.44140625" customWidth="1"/>
-    <col min="5891" max="5891" width="40.109375" customWidth="1"/>
+    <col min="5637" max="5637" width="25.7109375" customWidth="1"/>
+    <col min="5889" max="5889" width="9.140625" customWidth="1"/>
+    <col min="5890" max="5890" width="15.42578125" customWidth="1"/>
+    <col min="5891" max="5891" width="40.140625" customWidth="1"/>
     <col min="5892" max="5892" width="22" customWidth="1"/>
-    <col min="5893" max="5893" width="25.6640625" customWidth="1"/>
-    <col min="6145" max="6145" width="9.109375" customWidth="1"/>
-    <col min="6146" max="6146" width="15.44140625" customWidth="1"/>
-    <col min="6147" max="6147" width="40.109375" customWidth="1"/>
+    <col min="5893" max="5893" width="25.7109375" customWidth="1"/>
+    <col min="6145" max="6145" width="9.140625" customWidth="1"/>
+    <col min="6146" max="6146" width="15.42578125" customWidth="1"/>
+    <col min="6147" max="6147" width="40.140625" customWidth="1"/>
     <col min="6148" max="6148" width="22" customWidth="1"/>
-    <col min="6149" max="6149" width="25.6640625" customWidth="1"/>
-    <col min="6401" max="6401" width="9.109375" customWidth="1"/>
-    <col min="6402" max="6402" width="15.44140625" customWidth="1"/>
-    <col min="6403" max="6403" width="40.109375" customWidth="1"/>
+    <col min="6149" max="6149" width="25.7109375" customWidth="1"/>
+    <col min="6401" max="6401" width="9.140625" customWidth="1"/>
+    <col min="6402" max="6402" width="15.42578125" customWidth="1"/>
+    <col min="6403" max="6403" width="40.140625" customWidth="1"/>
     <col min="6404" max="6404" width="22" customWidth="1"/>
-    <col min="6405" max="6405" width="25.6640625" customWidth="1"/>
-    <col min="6657" max="6657" width="9.109375" customWidth="1"/>
-    <col min="6658" max="6658" width="15.44140625" customWidth="1"/>
-    <col min="6659" max="6659" width="40.109375" customWidth="1"/>
+    <col min="6405" max="6405" width="25.7109375" customWidth="1"/>
+    <col min="6657" max="6657" width="9.140625" customWidth="1"/>
+    <col min="6658" max="6658" width="15.42578125" customWidth="1"/>
+    <col min="6659" max="6659" width="40.140625" customWidth="1"/>
     <col min="6660" max="6660" width="22" customWidth="1"/>
-    <col min="6661" max="6661" width="25.6640625" customWidth="1"/>
-    <col min="6913" max="6913" width="9.109375" customWidth="1"/>
-    <col min="6914" max="6914" width="15.44140625" customWidth="1"/>
-    <col min="6915" max="6915" width="40.109375" customWidth="1"/>
+    <col min="6661" max="6661" width="25.7109375" customWidth="1"/>
+    <col min="6913" max="6913" width="9.140625" customWidth="1"/>
+    <col min="6914" max="6914" width="15.42578125" customWidth="1"/>
+    <col min="6915" max="6915" width="40.140625" customWidth="1"/>
     <col min="6916" max="6916" width="22" customWidth="1"/>
-    <col min="6917" max="6917" width="25.6640625" customWidth="1"/>
-    <col min="7169" max="7169" width="9.109375" customWidth="1"/>
-    <col min="7170" max="7170" width="15.44140625" customWidth="1"/>
-    <col min="7171" max="7171" width="40.109375" customWidth="1"/>
+    <col min="6917" max="6917" width="25.7109375" customWidth="1"/>
+    <col min="7169" max="7169" width="9.140625" customWidth="1"/>
+    <col min="7170" max="7170" width="15.42578125" customWidth="1"/>
+    <col min="7171" max="7171" width="40.140625" customWidth="1"/>
     <col min="7172" max="7172" width="22" customWidth="1"/>
-    <col min="7173" max="7173" width="25.6640625" customWidth="1"/>
-    <col min="7425" max="7425" width="9.109375" customWidth="1"/>
-    <col min="7426" max="7426" width="15.44140625" customWidth="1"/>
-    <col min="7427" max="7427" width="40.109375" customWidth="1"/>
+    <col min="7173" max="7173" width="25.7109375" customWidth="1"/>
+    <col min="7425" max="7425" width="9.140625" customWidth="1"/>
+    <col min="7426" max="7426" width="15.42578125" customWidth="1"/>
+    <col min="7427" max="7427" width="40.140625" customWidth="1"/>
     <col min="7428" max="7428" width="22" customWidth="1"/>
-    <col min="7429" max="7429" width="25.6640625" customWidth="1"/>
-    <col min="7681" max="7681" width="9.109375" customWidth="1"/>
-    <col min="7682" max="7682" width="15.44140625" customWidth="1"/>
-    <col min="7683" max="7683" width="40.109375" customWidth="1"/>
+    <col min="7429" max="7429" width="25.7109375" customWidth="1"/>
+    <col min="7681" max="7681" width="9.140625" customWidth="1"/>
+    <col min="7682" max="7682" width="15.42578125" customWidth="1"/>
+    <col min="7683" max="7683" width="40.140625" customWidth="1"/>
     <col min="7684" max="7684" width="22" customWidth="1"/>
-    <col min="7685" max="7685" width="25.6640625" customWidth="1"/>
-    <col min="7937" max="7937" width="9.109375" customWidth="1"/>
-    <col min="7938" max="7938" width="15.44140625" customWidth="1"/>
-    <col min="7939" max="7939" width="40.109375" customWidth="1"/>
+    <col min="7685" max="7685" width="25.7109375" customWidth="1"/>
+    <col min="7937" max="7937" width="9.140625" customWidth="1"/>
+    <col min="7938" max="7938" width="15.42578125" customWidth="1"/>
+    <col min="7939" max="7939" width="40.140625" customWidth="1"/>
     <col min="7940" max="7940" width="22" customWidth="1"/>
-    <col min="7941" max="7941" width="25.6640625" customWidth="1"/>
-    <col min="8193" max="8193" width="9.109375" customWidth="1"/>
-    <col min="8194" max="8194" width="15.44140625" customWidth="1"/>
-    <col min="8195" max="8195" width="40.109375" customWidth="1"/>
+    <col min="7941" max="7941" width="25.7109375" customWidth="1"/>
+    <col min="8193" max="8193" width="9.140625" customWidth="1"/>
+    <col min="8194" max="8194" width="15.42578125" customWidth="1"/>
+    <col min="8195" max="8195" width="40.140625" customWidth="1"/>
     <col min="8196" max="8196" width="22" customWidth="1"/>
-    <col min="8197" max="8197" width="25.6640625" customWidth="1"/>
-    <col min="8449" max="8449" width="9.109375" customWidth="1"/>
-    <col min="8450" max="8450" width="15.44140625" customWidth="1"/>
-    <col min="8451" max="8451" width="40.109375" customWidth="1"/>
+    <col min="8197" max="8197" width="25.7109375" customWidth="1"/>
+    <col min="8449" max="8449" width="9.140625" customWidth="1"/>
+    <col min="8450" max="8450" width="15.42578125" customWidth="1"/>
+    <col min="8451" max="8451" width="40.140625" customWidth="1"/>
     <col min="8452" max="8452" width="22" customWidth="1"/>
-    <col min="8453" max="8453" width="25.6640625" customWidth="1"/>
-    <col min="8705" max="8705" width="9.109375" customWidth="1"/>
-    <col min="8706" max="8706" width="15.44140625" customWidth="1"/>
-    <col min="8707" max="8707" width="40.109375" customWidth="1"/>
+    <col min="8453" max="8453" width="25.7109375" customWidth="1"/>
+    <col min="8705" max="8705" width="9.140625" customWidth="1"/>
+    <col min="8706" max="8706" width="15.42578125" customWidth="1"/>
+    <col min="8707" max="8707" width="40.140625" customWidth="1"/>
     <col min="8708" max="8708" width="22" customWidth="1"/>
-    <col min="8709" max="8709" width="25.6640625" customWidth="1"/>
-    <col min="8961" max="8961" width="9.109375" customWidth="1"/>
-    <col min="8962" max="8962" width="15.44140625" customWidth="1"/>
-    <col min="8963" max="8963" width="40.109375" customWidth="1"/>
+    <col min="8709" max="8709" width="25.7109375" customWidth="1"/>
+    <col min="8961" max="8961" width="9.140625" customWidth="1"/>
+    <col min="8962" max="8962" width="15.42578125" customWidth="1"/>
+    <col min="8963" max="8963" width="40.140625" customWidth="1"/>
     <col min="8964" max="8964" width="22" customWidth="1"/>
-    <col min="8965" max="8965" width="25.6640625" customWidth="1"/>
-    <col min="9217" max="9217" width="9.109375" customWidth="1"/>
-    <col min="9218" max="9218" width="15.44140625" customWidth="1"/>
-    <col min="9219" max="9219" width="40.109375" customWidth="1"/>
+    <col min="8965" max="8965" width="25.7109375" customWidth="1"/>
+    <col min="9217" max="9217" width="9.140625" customWidth="1"/>
+    <col min="9218" max="9218" width="15.42578125" customWidth="1"/>
+    <col min="9219" max="9219" width="40.140625" customWidth="1"/>
     <col min="9220" max="9220" width="22" customWidth="1"/>
-    <col min="9221" max="9221" width="25.6640625" customWidth="1"/>
-    <col min="9473" max="9473" width="9.109375" customWidth="1"/>
-    <col min="9474" max="9474" width="15.44140625" customWidth="1"/>
-    <col min="9475" max="9475" width="40.109375" customWidth="1"/>
+    <col min="9221" max="9221" width="25.7109375" customWidth="1"/>
+    <col min="9473" max="9473" width="9.140625" customWidth="1"/>
+    <col min="9474" max="9474" width="15.42578125" customWidth="1"/>
+    <col min="9475" max="9475" width="40.140625" customWidth="1"/>
     <col min="9476" max="9476" width="22" customWidth="1"/>
-    <col min="9477" max="9477" width="25.6640625" customWidth="1"/>
-    <col min="9729" max="9729" width="9.109375" customWidth="1"/>
-    <col min="9730" max="9730" width="15.44140625" customWidth="1"/>
-    <col min="9731" max="9731" width="40.109375" customWidth="1"/>
+    <col min="9477" max="9477" width="25.7109375" customWidth="1"/>
+    <col min="9729" max="9729" width="9.140625" customWidth="1"/>
+    <col min="9730" max="9730" width="15.42578125" customWidth="1"/>
+    <col min="9731" max="9731" width="40.140625" customWidth="1"/>
     <col min="9732" max="9732" width="22" customWidth="1"/>
-    <col min="9733" max="9733" width="25.6640625" customWidth="1"/>
-    <col min="9985" max="9985" width="9.109375" customWidth="1"/>
-    <col min="9986" max="9986" width="15.44140625" customWidth="1"/>
-    <col min="9987" max="9987" width="40.109375" customWidth="1"/>
+    <col min="9733" max="9733" width="25.7109375" customWidth="1"/>
+    <col min="9985" max="9985" width="9.140625" customWidth="1"/>
+    <col min="9986" max="9986" width="15.42578125" customWidth="1"/>
+    <col min="9987" max="9987" width="40.140625" customWidth="1"/>
     <col min="9988" max="9988" width="22" customWidth="1"/>
-    <col min="9989" max="9989" width="25.6640625" customWidth="1"/>
-    <col min="10241" max="10241" width="9.109375" customWidth="1"/>
-    <col min="10242" max="10242" width="15.44140625" customWidth="1"/>
-    <col min="10243" max="10243" width="40.109375" customWidth="1"/>
+    <col min="9989" max="9989" width="25.7109375" customWidth="1"/>
+    <col min="10241" max="10241" width="9.140625" customWidth="1"/>
+    <col min="10242" max="10242" width="15.42578125" customWidth="1"/>
+    <col min="10243" max="10243" width="40.140625" customWidth="1"/>
     <col min="10244" max="10244" width="22" customWidth="1"/>
-    <col min="10245" max="10245" width="25.6640625" customWidth="1"/>
-    <col min="10497" max="10497" width="9.109375" customWidth="1"/>
-    <col min="10498" max="10498" width="15.44140625" customWidth="1"/>
-    <col min="10499" max="10499" width="40.109375" customWidth="1"/>
+    <col min="10245" max="10245" width="25.7109375" customWidth="1"/>
+    <col min="10497" max="10497" width="9.140625" customWidth="1"/>
+    <col min="10498" max="10498" width="15.42578125" customWidth="1"/>
+    <col min="10499" max="10499" width="40.140625" customWidth="1"/>
     <col min="10500" max="10500" width="22" customWidth="1"/>
-    <col min="10501" max="10501" width="25.6640625" customWidth="1"/>
-    <col min="10753" max="10753" width="9.109375" customWidth="1"/>
-    <col min="10754" max="10754" width="15.44140625" customWidth="1"/>
-    <col min="10755" max="10755" width="40.109375" customWidth="1"/>
+    <col min="10501" max="10501" width="25.7109375" customWidth="1"/>
+    <col min="10753" max="10753" width="9.140625" customWidth="1"/>
+    <col min="10754" max="10754" width="15.42578125" customWidth="1"/>
+    <col min="10755" max="10755" width="40.140625" customWidth="1"/>
     <col min="10756" max="10756" width="22" customWidth="1"/>
-    <col min="10757" max="10757" width="25.6640625" customWidth="1"/>
-    <col min="11009" max="11009" width="9.109375" customWidth="1"/>
-    <col min="11010" max="11010" width="15.44140625" customWidth="1"/>
-    <col min="11011" max="11011" width="40.109375" customWidth="1"/>
+    <col min="10757" max="10757" width="25.7109375" customWidth="1"/>
+    <col min="11009" max="11009" width="9.140625" customWidth="1"/>
+    <col min="11010" max="11010" width="15.42578125" customWidth="1"/>
+    <col min="11011" max="11011" width="40.140625" customWidth="1"/>
     <col min="11012" max="11012" width="22" customWidth="1"/>
-    <col min="11013" max="11013" width="25.6640625" customWidth="1"/>
-    <col min="11265" max="11265" width="9.109375" customWidth="1"/>
-    <col min="11266" max="11266" width="15.44140625" customWidth="1"/>
-    <col min="11267" max="11267" width="40.109375" customWidth="1"/>
+    <col min="11013" max="11013" width="25.7109375" customWidth="1"/>
+    <col min="11265" max="11265" width="9.140625" customWidth="1"/>
+    <col min="11266" max="11266" width="15.42578125" customWidth="1"/>
+    <col min="11267" max="11267" width="40.140625" customWidth="1"/>
     <col min="11268" max="11268" width="22" customWidth="1"/>
-    <col min="11269" max="11269" width="25.6640625" customWidth="1"/>
-    <col min="11521" max="11521" width="9.109375" customWidth="1"/>
-    <col min="11522" max="11522" width="15.44140625" customWidth="1"/>
-    <col min="11523" max="11523" width="40.109375" customWidth="1"/>
+    <col min="11269" max="11269" width="25.7109375" customWidth="1"/>
+    <col min="11521" max="11521" width="9.140625" customWidth="1"/>
+    <col min="11522" max="11522" width="15.42578125" customWidth="1"/>
+    <col min="11523" max="11523" width="40.140625" customWidth="1"/>
     <col min="11524" max="11524" width="22" customWidth="1"/>
-    <col min="11525" max="11525" width="25.6640625" customWidth="1"/>
-    <col min="11777" max="11777" width="9.109375" customWidth="1"/>
-    <col min="11778" max="11778" width="15.44140625" customWidth="1"/>
-    <col min="11779" max="11779" width="40.109375" customWidth="1"/>
+    <col min="11525" max="11525" width="25.7109375" customWidth="1"/>
+    <col min="11777" max="11777" width="9.140625" customWidth="1"/>
+    <col min="11778" max="11778" width="15.42578125" customWidth="1"/>
+    <col min="11779" max="11779" width="40.140625" customWidth="1"/>
     <col min="11780" max="11780" width="22" customWidth="1"/>
-    <col min="11781" max="11781" width="25.6640625" customWidth="1"/>
-    <col min="12033" max="12033" width="9.109375" customWidth="1"/>
-    <col min="12034" max="12034" width="15.44140625" customWidth="1"/>
-    <col min="12035" max="12035" width="40.109375" customWidth="1"/>
+    <col min="11781" max="11781" width="25.7109375" customWidth="1"/>
+    <col min="12033" max="12033" width="9.140625" customWidth="1"/>
+    <col min="12034" max="12034" width="15.42578125" customWidth="1"/>
+    <col min="12035" max="12035" width="40.140625" customWidth="1"/>
     <col min="12036" max="12036" width="22" customWidth="1"/>
-    <col min="12037" max="12037" width="25.6640625" customWidth="1"/>
-    <col min="12289" max="12289" width="9.109375" customWidth="1"/>
-    <col min="12290" max="12290" width="15.44140625" customWidth="1"/>
-    <col min="12291" max="12291" width="40.109375" customWidth="1"/>
+    <col min="12037" max="12037" width="25.7109375" customWidth="1"/>
+    <col min="12289" max="12289" width="9.140625" customWidth="1"/>
+    <col min="12290" max="12290" width="15.42578125" customWidth="1"/>
+    <col min="12291" max="12291" width="40.140625" customWidth="1"/>
     <col min="12292" max="12292" width="22" customWidth="1"/>
-    <col min="12293" max="12293" width="25.6640625" customWidth="1"/>
-    <col min="12545" max="12545" width="9.109375" customWidth="1"/>
-    <col min="12546" max="12546" width="15.44140625" customWidth="1"/>
-    <col min="12547" max="12547" width="40.109375" customWidth="1"/>
+    <col min="12293" max="12293" width="25.7109375" customWidth="1"/>
+    <col min="12545" max="12545" width="9.140625" customWidth="1"/>
+    <col min="12546" max="12546" width="15.42578125" customWidth="1"/>
+    <col min="12547" max="12547" width="40.140625" customWidth="1"/>
     <col min="12548" max="12548" width="22" customWidth="1"/>
-    <col min="12549" max="12549" width="25.6640625" customWidth="1"/>
-    <col min="12801" max="12801" width="9.109375" customWidth="1"/>
-    <col min="12802" max="12802" width="15.44140625" customWidth="1"/>
-    <col min="12803" max="12803" width="40.109375" customWidth="1"/>
+    <col min="12549" max="12549" width="25.7109375" customWidth="1"/>
+    <col min="12801" max="12801" width="9.140625" customWidth="1"/>
+    <col min="12802" max="12802" width="15.42578125" customWidth="1"/>
+    <col min="12803" max="12803" width="40.140625" customWidth="1"/>
     <col min="12804" max="12804" width="22" customWidth="1"/>
-    <col min="12805" max="12805" width="25.6640625" customWidth="1"/>
-    <col min="13057" max="13057" width="9.109375" customWidth="1"/>
-    <col min="13058" max="13058" width="15.44140625" customWidth="1"/>
-    <col min="13059" max="13059" width="40.109375" customWidth="1"/>
+    <col min="12805" max="12805" width="25.7109375" customWidth="1"/>
+    <col min="13057" max="13057" width="9.140625" customWidth="1"/>
+    <col min="13058" max="13058" width="15.42578125" customWidth="1"/>
+    <col min="13059" max="13059" width="40.140625" customWidth="1"/>
     <col min="13060" max="13060" width="22" customWidth="1"/>
-    <col min="13061" max="13061" width="25.6640625" customWidth="1"/>
-    <col min="13313" max="13313" width="9.109375" customWidth="1"/>
-    <col min="13314" max="13314" width="15.44140625" customWidth="1"/>
-    <col min="13315" max="13315" width="40.109375" customWidth="1"/>
+    <col min="13061" max="13061" width="25.7109375" customWidth="1"/>
+    <col min="13313" max="13313" width="9.140625" customWidth="1"/>
+    <col min="13314" max="13314" width="15.42578125" customWidth="1"/>
+    <col min="13315" max="13315" width="40.140625" customWidth="1"/>
     <col min="13316" max="13316" width="22" customWidth="1"/>
-    <col min="13317" max="13317" width="25.6640625" customWidth="1"/>
-    <col min="13569" max="13569" width="9.109375" customWidth="1"/>
-    <col min="13570" max="13570" width="15.44140625" customWidth="1"/>
-    <col min="13571" max="13571" width="40.109375" customWidth="1"/>
+    <col min="13317" max="13317" width="25.7109375" customWidth="1"/>
+    <col min="13569" max="13569" width="9.140625" customWidth="1"/>
+    <col min="13570" max="13570" width="15.42578125" customWidth="1"/>
+    <col min="13571" max="13571" width="40.140625" customWidth="1"/>
     <col min="13572" max="13572" width="22" customWidth="1"/>
-    <col min="13573" max="13573" width="25.6640625" customWidth="1"/>
-    <col min="13825" max="13825" width="9.109375" customWidth="1"/>
-    <col min="13826" max="13826" width="15.44140625" customWidth="1"/>
-    <col min="13827" max="13827" width="40.109375" customWidth="1"/>
+    <col min="13573" max="13573" width="25.7109375" customWidth="1"/>
+    <col min="13825" max="13825" width="9.140625" customWidth="1"/>
+    <col min="13826" max="13826" width="15.42578125" customWidth="1"/>
+    <col min="13827" max="13827" width="40.140625" customWidth="1"/>
     <col min="13828" max="13828" width="22" customWidth="1"/>
-    <col min="13829" max="13829" width="25.6640625" customWidth="1"/>
-    <col min="14081" max="14081" width="9.109375" customWidth="1"/>
-    <col min="14082" max="14082" width="15.44140625" customWidth="1"/>
-    <col min="14083" max="14083" width="40.109375" customWidth="1"/>
+    <col min="13829" max="13829" width="25.7109375" customWidth="1"/>
+    <col min="14081" max="14081" width="9.140625" customWidth="1"/>
+    <col min="14082" max="14082" width="15.42578125" customWidth="1"/>
+    <col min="14083" max="14083" width="40.140625" customWidth="1"/>
     <col min="14084" max="14084" width="22" customWidth="1"/>
-    <col min="14085" max="14085" width="25.6640625" customWidth="1"/>
-    <col min="14337" max="14337" width="9.109375" customWidth="1"/>
-    <col min="14338" max="14338" width="15.44140625" customWidth="1"/>
-    <col min="14339" max="14339" width="40.109375" customWidth="1"/>
+    <col min="14085" max="14085" width="25.7109375" customWidth="1"/>
+    <col min="14337" max="14337" width="9.140625" customWidth="1"/>
+    <col min="14338" max="14338" width="15.42578125" customWidth="1"/>
+    <col min="14339" max="14339" width="40.140625" customWidth="1"/>
     <col min="14340" max="14340" width="22" customWidth="1"/>
-    <col min="14341" max="14341" width="25.6640625" customWidth="1"/>
-    <col min="14593" max="14593" width="9.109375" customWidth="1"/>
-    <col min="14594" max="14594" width="15.44140625" customWidth="1"/>
-    <col min="14595" max="14595" width="40.109375" customWidth="1"/>
+    <col min="14341" max="14341" width="25.7109375" customWidth="1"/>
+    <col min="14593" max="14593" width="9.140625" customWidth="1"/>
+    <col min="14594" max="14594" width="15.42578125" customWidth="1"/>
+    <col min="14595" max="14595" width="40.140625" customWidth="1"/>
     <col min="14596" max="14596" width="22" customWidth="1"/>
-    <col min="14597" max="14597" width="25.6640625" customWidth="1"/>
-    <col min="14849" max="14849" width="9.109375" customWidth="1"/>
-    <col min="14850" max="14850" width="15.44140625" customWidth="1"/>
-    <col min="14851" max="14851" width="40.109375" customWidth="1"/>
+    <col min="14597" max="14597" width="25.7109375" customWidth="1"/>
+    <col min="14849" max="14849" width="9.140625" customWidth="1"/>
+    <col min="14850" max="14850" width="15.42578125" customWidth="1"/>
+    <col min="14851" max="14851" width="40.140625" customWidth="1"/>
     <col min="14852" max="14852" width="22" customWidth="1"/>
-    <col min="14853" max="14853" width="25.6640625" customWidth="1"/>
-    <col min="15105" max="15105" width="9.109375" customWidth="1"/>
-    <col min="15106" max="15106" width="15.44140625" customWidth="1"/>
-    <col min="15107" max="15107" width="40.109375" customWidth="1"/>
+    <col min="14853" max="14853" width="25.7109375" customWidth="1"/>
+    <col min="15105" max="15105" width="9.140625" customWidth="1"/>
+    <col min="15106" max="15106" width="15.42578125" customWidth="1"/>
+    <col min="15107" max="15107" width="40.140625" customWidth="1"/>
     <col min="15108" max="15108" width="22" customWidth="1"/>
-    <col min="15109" max="15109" width="25.6640625" customWidth="1"/>
-    <col min="15361" max="15361" width="9.109375" customWidth="1"/>
-    <col min="15362" max="15362" width="15.44140625" customWidth="1"/>
-    <col min="15363" max="15363" width="40.109375" customWidth="1"/>
+    <col min="15109" max="15109" width="25.7109375" customWidth="1"/>
+    <col min="15361" max="15361" width="9.140625" customWidth="1"/>
+    <col min="15362" max="15362" width="15.42578125" customWidth="1"/>
+    <col min="15363" max="15363" width="40.140625" customWidth="1"/>
     <col min="15364" max="15364" width="22" customWidth="1"/>
-    <col min="15365" max="15365" width="25.6640625" customWidth="1"/>
-    <col min="15617" max="15617" width="9.109375" customWidth="1"/>
-    <col min="15618" max="15618" width="15.44140625" customWidth="1"/>
-    <col min="15619" max="15619" width="40.109375" customWidth="1"/>
+    <col min="15365" max="15365" width="25.7109375" customWidth="1"/>
+    <col min="15617" max="15617" width="9.140625" customWidth="1"/>
+    <col min="15618" max="15618" width="15.42578125" customWidth="1"/>
+    <col min="15619" max="15619" width="40.140625" customWidth="1"/>
     <col min="15620" max="15620" width="22" customWidth="1"/>
-    <col min="15621" max="15621" width="25.6640625" customWidth="1"/>
-    <col min="15873" max="15873" width="9.109375" customWidth="1"/>
-    <col min="15874" max="15874" width="15.44140625" customWidth="1"/>
-    <col min="15875" max="15875" width="40.109375" customWidth="1"/>
+    <col min="15621" max="15621" width="25.7109375" customWidth="1"/>
+    <col min="15873" max="15873" width="9.140625" customWidth="1"/>
+    <col min="15874" max="15874" width="15.42578125" customWidth="1"/>
+    <col min="15875" max="15875" width="40.140625" customWidth="1"/>
     <col min="15876" max="15876" width="22" customWidth="1"/>
-    <col min="15877" max="15877" width="25.6640625" customWidth="1"/>
-    <col min="16129" max="16129" width="9.109375" customWidth="1"/>
-    <col min="16130" max="16130" width="15.44140625" customWidth="1"/>
-    <col min="16131" max="16131" width="40.109375" customWidth="1"/>
+    <col min="15877" max="15877" width="25.7109375" customWidth="1"/>
+    <col min="16129" max="16129" width="9.140625" customWidth="1"/>
+    <col min="16130" max="16130" width="15.42578125" customWidth="1"/>
+    <col min="16131" max="16131" width="40.140625" customWidth="1"/>
     <col min="16132" max="16132" width="22" customWidth="1"/>
-    <col min="16133" max="16133" width="25.6640625" customWidth="1"/>
+    <col min="16133" max="16133" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
         <v>42255</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="11">
         <v>1</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="26.4" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
         <v>42451</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="11">
         <v>1.01</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
         <v>43122</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="11">
         <v>1.02</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
         <v>43123</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="11">
         <v>1.03</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="39.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <v>43129</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="11">
         <v>1.04</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <v>43224</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="11">
         <v>1.05</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <v>43580</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="11">
+        <v>1.06</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="9"/>
       <c r="D12" s="11"/>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="11"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="11"/>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="9"/>
       <c r="D15" s="11"/>
       <c r="E15" s="10"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
       <c r="D16" s="11"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
       <c r="D17" s="11"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
       <c r="D18" s="11"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="11"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="11"/>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
       <c r="D21" s="11"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="C22" s="9"/>
       <c r="D22" s="11"/>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="11"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
       <c r="D24" s="11"/>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="11"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="C26" s="9"/>
       <c r="D26" s="11"/>
       <c r="E26" s="10"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="11"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="12"/>
       <c r="C28" s="7"/>
       <c r="D28" s="11"/>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="C29" s="9"/>
       <c r="D29" s="11"/>
       <c r="E29" s="10"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="12"/>
       <c r="C30" s="9"/>
       <c r="D30" s="11"/>
       <c r="E30" s="10"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
       <c r="D31" s="11"/>
       <c r="E31" s="10"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="12"/>
       <c r="D32" s="11"/>
       <c r="E32" s="10"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="12"/>
       <c r="D33" s="11"/>
       <c r="E33" s="10"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="12"/>
       <c r="C34" s="13"/>
       <c r="D34" s="11"/>
       <c r="E34" s="10"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="12"/>
       <c r="D35" s="11"/>
       <c r="E35" s="10"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="12"/>
       <c r="D36" s="11"/>
       <c r="E36" s="10"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="12"/>
       <c r="D37" s="11"/>
       <c r="E37" s="10"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="12"/>
       <c r="D38" s="11"/>
       <c r="E38" s="10"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="12"/>
       <c r="D39" s="11"/>
       <c r="E39" s="10"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="12"/>
       <c r="D40" s="11"/>
       <c r="E40" s="10"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="12"/>
       <c r="C41" s="13"/>
       <c r="D41" s="11"/>
       <c r="E41" s="10"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="12"/>
       <c r="C42" s="13"/>
       <c r="D42" s="11"/>
       <c r="E42" s="10"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="12"/>
       <c r="D43" s="11"/>
       <c r="E43" s="10"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="12"/>
       <c r="D44" s="11"/>
       <c r="E44" s="10"/>
     </row>
-    <row r="45" spans="2:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="12"/>
       <c r="D45" s="11"/>
       <c r="E45" s="10"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="12"/>
       <c r="D46" s="11"/>
       <c r="E46" s="10"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="12"/>
       <c r="D47" s="11"/>
       <c r="E47" s="10"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="12"/>
       <c r="D48" s="11"/>
       <c r="E48" s="10"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="12"/>
       <c r="D49" s="11"/>
       <c r="E49" s="10"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="12"/>
       <c r="D50" s="11"/>
       <c r="E50" s="10"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="12"/>
       <c r="D51" s="11"/>
       <c r="E51" s="10"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="12"/>
       <c r="D52" s="11"/>
       <c r="E52" s="10"/>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="12"/>
       <c r="D53" s="11"/>
       <c r="E53" s="10"/>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="12"/>
       <c r="D54" s="11"/>
       <c r="E54" s="10"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="12"/>
       <c r="D55" s="11"/>
       <c r="E55" s="10"/>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="12"/>
       <c r="D56" s="11"/>
       <c r="E56" s="10"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="12"/>
       <c r="D57" s="11"/>
       <c r="E57" s="10"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="12"/>
       <c r="D58" s="11"/>
       <c r="E58" s="10"/>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="12"/>
       <c r="D59" s="11"/>
       <c r="E59" s="10"/>
@@ -1298,34 +1327,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" customWidth="1"/>
-    <col min="9" max="9" width="26.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>0</v>
@@ -1343,27 +1372,27 @@
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="L1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1384,7 +1413,7 @@
         <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
@@ -1396,12 +1425,12 @@
         <v>42255</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -1416,13 +1445,13 @@
         <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
         <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
@@ -1434,12 +1463,12 @@
         <v>42255</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -1454,13 +1483,13 @@
         <v>16</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J4" t="s">
         <v>18</v>
@@ -1472,24 +1501,24 @@
         <v>42255</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>13</v>
@@ -1498,7 +1527,7 @@
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J5" t="s">
         <v>18</v>
@@ -1510,18 +1539,18 @@
         <v>42255</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -1536,7 +1565,7 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J6" t="s">
         <v>18</v>
@@ -1548,24 +1577,24 @@
         <v>42255</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>13</v>
@@ -1574,7 +1603,7 @@
         <v>4</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>18</v>
@@ -1589,47 +1618,53 @@
         <v>43224</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2">
         <v>98</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>19</v>
+      <c r="D8" t="s">
+        <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="J8" t="s">
         <v>4</v>
       </c>
       <c r="K8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="L8" s="12">
+        <v>43586</v>
+      </c>
+      <c r="M8" s="12">
+        <v>43647</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2">
         <v>99</v>
@@ -1650,7 +1685,7 @@
         <v>4</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J9" t="s">
         <v>18</v>
@@ -1674,7 +1709,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
20256 - ecl qn survey
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C48999
</commit_message>
<xml_diff>
--- a/Requirements/CCO_eCoaching_Log_Survey_Questions.xlsx
+++ b/Requirements/CCO_eCoaching_Log_Survey_Questions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian.coughlin\Documents\TFS\OY6\Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS_Omni\eCoaching_V2\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8F3BC2-4888-48AA-A70D-4A879256DE90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="1"/>
+    <workbookView xWindow="5565" yWindow="1335" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="2" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="56">
   <si>
     <t>Survey Question</t>
   </si>
@@ -189,9 +190,6 @@
 set active to No and end date to 05/04/2018</t>
   </si>
   <si>
-    <t>London</t>
-  </si>
-  <si>
     <t>Quality Now has improved my experience working on the CCO</t>
   </si>
   <si>
@@ -212,11 +210,20 @@
   <si>
     <t>TFS14209 - eCoaching - Add new Hot Topic Survey question 5/1-7/1/2019</t>
   </si>
+  <si>
+    <t>Chester, Hattiesburg, London, Lynn Haven, Tampa, Winchester,</t>
+  </si>
+  <si>
+    <t>tfs20256 - ecl qn surverys - phase ii sites</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -401,6 +408,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -436,6 +460,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -611,11 +652,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,20 +1086,28 @@
         <v>43580</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="11">
         <v>1.06</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="10"/>
+      <c r="B12" s="6">
+        <v>44286</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="11">
+        <v>1.07</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
@@ -1324,11 +1373,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,20 +1671,20 @@
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
-        <v>48</v>
+      <c r="B8" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C8" s="2">
         <v>98</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>13</v>
@@ -1644,7 +1693,7 @@
         <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J8" t="s">
         <v>4</v>
@@ -1655,8 +1704,8 @@
       <c r="L8" s="12">
         <v>43586</v>
       </c>
-      <c r="M8" s="12">
-        <v>43647</v>
+      <c r="M8" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1704,7 +1753,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>